<commit_message>
finish some quest data
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17571"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,42 +14,12 @@
   <sheets>
     <sheet name="Quest" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="56">
-  <si>
-    <t>开始</t>
-  </si>
-  <si>
-    <t>血蓟药</t>
-  </si>
-  <si>
-    <t>乔斯基叔叔说血蓟是一种神奇的草药，希望我可以帮他采集三个。</t>
-  </si>
-  <si>
-    <t>奖励</t>
-  </si>
-  <si>
-    <t>乔斯基叔叔让我去找铁匠，说铁匠已经为给我准备了一些装备。</t>
-  </si>
-  <si>
-    <t>鼠患</t>
-  </si>
-  <si>
-    <t>乔斯基叔叔表示房子阁楼里充满了许许多多的老鼠，希望我可以帮助赶走这些老鼠。</t>
-  </si>
-  <si>
-    <t>令牌</t>
-  </si>
-  <si>
-    <t>乔斯基叔叔说要我帮他找到一块皇城令牌，也不知道是干啥用的。</t>
-  </si>
-  <si>
-    <t>东方女子</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="72">
   <si>
     <t>东方商人和我讲述了他来到这里的故事，并告诉我他曾经认识一位来自东方的召唤师。</t>
   </si>
@@ -137,10 +107,6 @@
     <t>Descript</t>
   </si>
   <si>
-    <t>乔斯基叔叔和我说了很多以前的故事，并希望我可以从今天开始修行。但是首先需要选择一把属于自己的武器。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>12000001|Start</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -208,14 +174,115 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>piece</t>
+    <t>传说</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcqiaosiji</t>
+  </si>
+  <si>
+    <t>乔斯基是你的叔叔，他为你讲述了一个传奇的故事</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>|在我成年礼的那天，一早我去拜访了|G|乔斯基叔叔||，他说为了准备了一份成年礼物。到了叔叔家，乔斯基给我讲述一个古老的故事。$|故事就发生在|B|塔塔木森林||的更北面。很久以前，有一位大陆上都非常有名的勇士离开|B|塔塔木村||，但是却误入了这片森林。勇士心中丝毫没有一点害怕，他的勇武使他充满了自信。就这样，在迷路的情况下，他一直向北走了两天，直到一座高塔挡住了他的去路。这其实就是传说中的|B|布萨特高塔||，一个通过历练就可以大大提升自己能力的地方。勇士当时并不知情，他当时毫不犹豫的进入了高塔，希望可以有所收获。。。从此，关于这位勇士就销声匿迹了，世界上再也没有关于他的传说。$$|乔斯基希望你可以找到|B|布萨特高塔||，并到其中锻炼自己。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcsainisi</t>
+  </si>
+  <si>
+    <t>qiongqi</t>
+  </si>
+  <si>
+    <t>龙眼塞尼斯，是一位卡牌召唤师，传说具有与龙沟通的能力</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>穷奇是一种传说的远古神兽，非常凶残</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>|就这样，我离开了自己的家，开始远行，寻找|B|布萨特高塔||。这个地方真的存在吗，或是如果存在，我真的能够找到吗，我完全没有把握。我决定先到达|B|塔塔木村||，那里说不定会有人可以给我一些信息。$B|昏暗密林||到往|B|塔塔木村||的必经之路。我对这片密林已经非常熟悉，从小时候就时常和叔叔一同在林间捕猎。虽然，林子中的狼偶尔会给我们带来一些麻烦。这次，我在林间偶然遇到了|G|塞尼斯||，他的右眼非常像龙的眼睛，并自称具有和龙沟通的能力。他说，经过几天的追踪，他发现了远古神兽|R|穷奇||的踪迹，并提出如果能够战胜他，就可以和他一同进入|B|密林深处|对决神兽。$|对决中，我利用法术渡过了前期的猛攻，后期利用|P|作战傀儡||加上强化法术，一波流带走对手。我的能力完全超出了|G|塞尼斯||的预想，他也同意了带我一起进入密林。$|这片森林处处充满着诡异的气氛，来回几次，我们发现自己只是在原地打转。偶然间，我们发现了森林的秘密，原来只有按照一定的顺序才能走出这个迷宫。而在迷宫尽头，我们找到了|R|穷奇||，一场大战看来已经不可避免。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcsaibasi</t>
+  </si>
+  <si>
+    <t>塞巴斯恰恩欺骗你重伤了科迪，他到底意欲何为</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>田园的守护者，他其实是为了守护主人所在的古城</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcaolai</t>
+  </si>
+  <si>
+    <t>欺骗</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>四骑士</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npckedi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcmilanda</t>
+  </si>
+  <si>
+    <t>科迪就像一个暴力的猩猩，不让你靠近峡谷的深处</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>钥匙</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>黑暗之门</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>神兽穷奇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>|虽然很担忧古城那边的情况，但我还是决定现寻找高塔。果然，我非常顺利的经由|B|小树林||进入了|B|登拉克峡谷||。在峡谷中我发现了一处村落的遗迹，似乎已经荒废很多年了。进入到峡谷中心地带区域，我遇到了|G|科迪||，他就像是一只野蛮的猩猩，拦住了我的去路，并声称只能从他的尸体上过去。我只好照做，峡谷深处一直往里走，我进入到了一个山洞中。$|在漆黑的洞穴中一直走了半天时间，我发现自己竟然已经身处|B|玲珑峰||顶部。继续往里走，我吃惊地发现，我已经可以远远望见高塔了。就在这时，|G|米兰达||现身了，她说，他和|G|科迪||、|G|奥莱伊李||、|G|塞巴斯恰恩||曾经是“天启四骑士”。他们使用各种办法不让外人靠近|B|布萨特高塔||，而你可以到达这一关，已经是非常了不起了。|G|米兰达||并表示，我必须先找到三件道具，才可以进入高塔，否则也是打不开高塔的大门的。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>米兰达作为高塔前最后的守护者，要求我找到三件道具，才能进入高塔</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>|击败了远古神兽之后，我和|G|塞尼斯||分道扬镳，他说我们总有一天会再一决高下。来到|B|塔塔木村||之后，我并没能够获得一些关于高塔有用的信息。于是，在进行了简单的补给之后，我只好继续往北走，进入|B|小树林||。|B|小树林||确实如其名，是一片很小的树林，但却是到达|B|登拉克峡谷||的必经之路。而后者是却被广阔的神秘森林所覆盖，很有可能隐藏了通往高塔的去路。|B|小树林||中我遇到了|G|塞巴斯恰恩||，在帮他解决了麻烦之后，他告诉我因为前几天的大雨，通往峡谷的道路已经被冲毁，现在只能绕道|B|村外田园||的小路过去。$|谢过他之后，我转到到达|B|村外田园||。但是这里的管家|G|奥莱伊李||却非常傲慢无礼，不管我如何解释，他不让我进入田园，并坚持这里没有通往高塔的道路。在我通过卡牌对决重伤|G|奥莱伊李||后，他终于说出了缘由。田园其实是一条通往|B|珀斯古城||的要道，而它的主人要他坚守于此，不让任何人进入。$|我终于意识到自己被欺骗了，就在我回去追问|G|塞巴斯恰恩||之时，他声称此时一群匪贼通过田园进入了古城，失去了|G|奥莱伊李||守护的田园，任何人都可以随意进出。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>米兰达需要我找到三把钥匙</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcweia</t>
+  </si>
+  <si>
+    <t>威阿伊丁自称这里的国王，整个人疯疯癫癫的</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>|让我非常吃惊的是，|G|米兰达||告诉我那三件道具其实是三把钥匙。|Y|智慧钥匙||、|Y|力量钥匙||、|Y|勇气钥匙||，这三把钥匙拼接在一起开启|B|布萨特高塔||的大门。在|G|米兰达||的帮助下，我先后获得了|Y|智慧钥匙||、|Y|力量钥匙||。但是|Y|勇气钥匙||却被存放在|B|珀斯古城||的最深处。看来我还是必须去一趟古城，去找寻这最后一把钥匙。$|在古城门口，我遇到了|G|威阿伊丁||，他要求所有人都对他施已王室的敬礼。他说他是这片王城的国王，但是战乱毁了这里，仅仅留下一片废墟。但是，我可以感觉到，他的神志并不是很正常，还是不要和他多做纠缠为好。$|古城内完全是一个黑暗的世界，这里的亡灵生物非常多，并且力量非常强大。通过层层的阻拦，我终于到达了最深处，并找到了传说中的|Y|勇气钥匙||。</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -901,63 +968,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -984,13 +995,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1005,7 +1009,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:K18" totalsRowShown="0" headerRowDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:K18" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A3:K18"/>
   <sortState ref="A4:AD60">
     <sortCondition ref="A3:A60"/>
@@ -1028,7 +1032,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1103,6 +1107,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1138,6 +1159,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1316,8 +1354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1330,115 +1368,115 @@
   <sheetData>
     <row r="1" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>42</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="I3" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="K3" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1447,25 +1485,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="G4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J4" t="s">
-        <v>55</v>
-      </c>
-      <c r="K4" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
@@ -1473,7 +1499,7 @@
         <v>12000002</v>
       </c>
       <c r="B5" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1482,25 +1508,19 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="G5" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="I5" t="s">
-        <v>54</v>
-      </c>
-      <c r="J5" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
@@ -1508,7 +1528,7 @@
         <v>12000003</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1517,7 +1537,7 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>67</v>
       </c>
       <c r="F6" t="s">
         <v>53</v>
@@ -1526,16 +1546,10 @@
         <v>54</v>
       </c>
       <c r="H6" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="I6" t="s">
-        <v>54</v>
-      </c>
-      <c r="J6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
@@ -1543,7 +1557,7 @@
         <v>12000004</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1552,25 +1566,19 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>6</v>
+        <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G7" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="H7" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="I7" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" t="s">
-        <v>53</v>
-      </c>
-      <c r="K7" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
@@ -1578,7 +1586,7 @@
         <v>12000005</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1587,25 +1595,19 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="F8" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="H8" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
       <c r="I8" t="s">
-        <v>54</v>
-      </c>
-      <c r="J8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K8" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
@@ -1613,7 +1615,7 @@
         <v>12000006</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1622,25 +1624,25 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F9" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G9" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H9" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="I9" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K9" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
@@ -1648,7 +1650,7 @@
         <v>12000007</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1657,25 +1659,25 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G10" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H10" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="I10" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J10" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K10" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.15">
@@ -1683,7 +1685,7 @@
         <v>12000008</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1692,25 +1694,25 @@
         <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H11" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="I11" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J11" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K11" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.15">
@@ -1718,7 +1720,7 @@
         <v>12000009</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1727,25 +1729,25 @@
         <v>9</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H12" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="I12" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J12" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K12" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.15">
@@ -1753,7 +1755,7 @@
         <v>12000051</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1762,25 +1764,25 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="F13" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G13" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H13" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="I13" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J13" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K13" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.15">
@@ -1788,7 +1790,7 @@
         <v>12000052</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -1797,25 +1799,25 @@
         <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G14" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H14" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="I14" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J14" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K14" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.15">
@@ -1823,7 +1825,7 @@
         <v>12000053</v>
       </c>
       <c r="B15" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -1832,25 +1834,25 @@
         <v>3</v>
       </c>
       <c r="E15" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G15" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H15" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="I15" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J15" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K15" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.15">
@@ -1858,7 +1860,7 @@
         <v>12000054</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1867,25 +1869,25 @@
         <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="I16" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J16" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K16" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.15">
@@ -1893,7 +1895,7 @@
         <v>12010004</v>
       </c>
       <c r="B17" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -1902,25 +1904,25 @@
         <v>5</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G17" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H17" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="I17" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J17" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K17" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.15">
@@ -1928,7 +1930,7 @@
         <v>12010005</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1937,31 +1939,31 @@
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="F18" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G18" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="H18" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="I18" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="J18" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="K18" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="A4:K18">
-    <cfRule type="containsBlanks" dxfId="10" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
finish the quest data and newbie quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -19,65 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="72">
-  <si>
-    <t>东方商人和我讲述了他来到这里的故事，并告诉我他曾经认识一位来自东方的召唤师。</t>
-  </si>
-  <si>
-    <t>第一个对手</t>
-  </si>
-  <si>
-    <t>终于遇到了我的第一个对手，发挥实力战胜她吧。</t>
-  </si>
-  <si>
-    <t>叔叔的身世</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="56">
   <si>
     <t>铁匠和我说了很多关于我叔叔以前的故事，原来他曾经是一个十分厉害的卡片召唤师。</t>
   </si>
   <si>
-    <t>目标</t>
-  </si>
-  <si>
-    <t>当我知道叔叔的事后，向叔叔发誓要更加努力的提高自己。</t>
-  </si>
-  <si>
-    <t>大扫除</t>
-  </si>
-  <si>
-    <t>乔斯基希望我去后院入口内，击败其中怪物3次。</t>
-  </si>
-  <si>
-    <t>红宝石</t>
-  </si>
-  <si>
-    <t>乔斯基希望我可以搞到一些红宝石。</t>
-  </si>
-  <si>
-    <t>收集</t>
-  </si>
-  <si>
-    <t>乔斯基叔叔表示玛莎是一个好的对手，可以通过战胜使自己变得更强。</t>
-  </si>
-  <si>
-    <t>勇士</t>
-  </si>
-  <si>
-    <t>乔斯基叔叔表示如果你可以击败玛莎20次，他会给你一份礼物。</t>
-  </si>
-  <si>
-    <t>共和国之剑</t>
-  </si>
-  <si>
-    <t>乔斯基叔叔让我去找维克多学习一些战斗的技巧，然后去村子北部进行探险历练。</t>
-  </si>
-  <si>
-    <t>龙之眼</t>
-  </si>
-  <si>
-    <t>塞尼斯莫名地提出与我决斗。</t>
-  </si>
-  <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -276,6 +222,14 @@
   </si>
   <si>
     <t>|让我非常吃惊的是，|G|米兰达||告诉我那三件道具其实是三把钥匙。|Y|智慧钥匙||、|Y|力量钥匙||、|Y|勇气钥匙||，这三把钥匙拼接在一起开启|B|布萨特高塔||的大门。在|G|米兰达||的帮助下，我先后获得了|Y|智慧钥匙||、|Y|力量钥匙||。但是|Y|勇气钥匙||却被存放在|B|珀斯古城||的最深处。看来我还是必须去一趟古城，去找寻这最后一把钥匙。$|在古城门口，我遇到了|G|威阿伊丁||，他要求所有人都对他施已王室的敬礼。他说他是这片王城的国王，但是战乱毁了这里，仅仅留下一片废墟。但是，我可以感觉到，他的神志并不是很正常，还是不要和他多做纠缠为好。$|古城内完全是一个黑暗的世界，这里的亡灵生物非常多，并且力量非常强大。通过层层的阻拦，我终于到达了最深处，并找到了传说中的|Y|勇气钥匙||。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>|通过三把钥匙，我打开了高塔的大门，一切的谜题感觉就要在今天解开了。那我传说中的的勇士在塔内究竟找到了什么？高塔第一层都是一些关于塔历史的壁画，似乎没有什么奇怪的东西。找到阶梯后，我就进入到了第二层，这里充满了各种机关，并且从机关的类型看来，年代并不是非常久远。我开始怀疑这个塔从何而来，这里并不像一个古代文明的古迹。奇怪的是，越是接近塔顶，这里黑暗的力量就越强大。终于，我来到了塔顶，在这里发现了一扇异世界的传送门，而所有黑暗力量的怪物都是由此而来。再消灭了从门内出现的一批怪物后，我赶紧破坏掉了传送门。一切都结束了吗？</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>海滩</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1009,10 +963,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:K18" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A3:K18"/>
-  <sortState ref="A4:AD60">
-    <sortCondition ref="A3:A60"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:K10" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A3:K10"/>
+  <sortState ref="A4:AD52">
+    <sortCondition ref="A3:A52"/>
   </sortState>
   <tableColumns count="11">
     <tableColumn id="1" name="Id"/>
@@ -1352,10 +1306,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1368,115 +1322,115 @@
   <sheetData>
     <row r="1" spans="1:11" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1485,13 +1439,13 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="G4" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.15">
@@ -1499,7 +1453,7 @@
         <v>12000002</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1508,19 +1462,19 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="H5" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.15">
@@ -1528,7 +1482,7 @@
         <v>12000003</v>
       </c>
       <c r="B6" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -1537,19 +1491,19 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="F6" t="s">
-        <v>53</v>
+        <v>35</v>
       </c>
       <c r="G6" t="s">
-        <v>54</v>
+        <v>36</v>
       </c>
       <c r="H6" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="I6" t="s">
-        <v>55</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.15">
@@ -1557,7 +1511,7 @@
         <v>12000004</v>
       </c>
       <c r="B7" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1566,19 +1520,19 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
       <c r="F7" t="s">
-        <v>59</v>
+        <v>41</v>
       </c>
       <c r="G7" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="H7" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
@@ -1586,7 +1540,7 @@
         <v>12000005</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -1595,19 +1549,19 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="F8" t="s">
-        <v>60</v>
+        <v>42</v>
       </c>
       <c r="G8" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="I8" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
@@ -1615,7 +1569,7 @@
         <v>12000006</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1624,345 +1578,47 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" t="s">
-        <v>43</v>
-      </c>
-      <c r="H9" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" t="s">
-        <v>43</v>
-      </c>
-      <c r="J9" t="s">
-        <v>42</v>
-      </c>
-      <c r="K9" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10">
-        <v>12000007</v>
+        <v>12001001</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="G10" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="H10" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="I10" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="J10" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="K10" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A11">
-        <v>12000008</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11">
-        <v>2</v>
-      </c>
-      <c r="D11">
-        <v>8</v>
-      </c>
-      <c r="E11" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" t="s">
-        <v>43</v>
-      </c>
-      <c r="H11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" t="s">
-        <v>43</v>
-      </c>
-      <c r="J11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A12">
-        <v>12000009</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>2</v>
-      </c>
-      <c r="D12">
-        <v>9</v>
-      </c>
-      <c r="E12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" t="s">
-        <v>42</v>
-      </c>
-      <c r="I12" t="s">
-        <v>43</v>
-      </c>
-      <c r="J12" t="s">
-        <v>42</v>
-      </c>
-      <c r="K12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A13">
-        <v>12000051</v>
-      </c>
-      <c r="B13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13">
-        <v>1</v>
-      </c>
-      <c r="E13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" t="s">
-        <v>43</v>
-      </c>
-      <c r="H13" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" t="s">
-        <v>43</v>
-      </c>
-      <c r="J13" t="s">
-        <v>42</v>
-      </c>
-      <c r="K13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A14">
-        <v>12000052</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14">
-        <v>2</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" t="s">
-        <v>43</v>
-      </c>
-      <c r="H14" t="s">
-        <v>42</v>
-      </c>
-      <c r="I14" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14" t="s">
-        <v>42</v>
-      </c>
-      <c r="K14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A15">
-        <v>12000053</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15">
-        <v>2</v>
-      </c>
-      <c r="D15">
-        <v>3</v>
-      </c>
-      <c r="E15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" t="s">
-        <v>42</v>
-      </c>
-      <c r="G15" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" t="s">
-        <v>42</v>
-      </c>
-      <c r="I15" t="s">
-        <v>43</v>
-      </c>
-      <c r="J15" t="s">
-        <v>42</v>
-      </c>
-      <c r="K15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A16">
-        <v>12000054</v>
-      </c>
-      <c r="B16" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
-        <v>4</v>
-      </c>
-      <c r="E16" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" t="s">
-        <v>42</v>
-      </c>
-      <c r="G16" t="s">
-        <v>43</v>
-      </c>
-      <c r="H16" t="s">
-        <v>42</v>
-      </c>
-      <c r="I16" t="s">
-        <v>43</v>
-      </c>
-      <c r="J16" t="s">
-        <v>42</v>
-      </c>
-      <c r="K16" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A17">
-        <v>12010004</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17">
-        <v>5</v>
-      </c>
-      <c r="E17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" t="s">
-        <v>43</v>
-      </c>
-      <c r="H17" t="s">
-        <v>42</v>
-      </c>
-      <c r="I17" t="s">
-        <v>43</v>
-      </c>
-      <c r="J17" t="s">
-        <v>42</v>
-      </c>
-      <c r="K17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.15">
-      <c r="A18">
-        <v>12010005</v>
-      </c>
-      <c r="B18" t="s">
-        <v>17</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" t="s">
-        <v>43</v>
-      </c>
-      <c r="H18" t="s">
-        <v>42</v>
-      </c>
-      <c r="I18" t="s">
-        <v>43</v>
-      </c>
-      <c r="J18" t="s">
-        <v>42</v>
-      </c>
-      <c r="K18" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="A4:K18">
+  <conditionalFormatting sqref="A4:K10">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>

</xml_diff>

<commit_message>
fill the scenequest info
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Quest" sheetId="1" r:id="rId1"/>
@@ -198,10 +198,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>|虽然很担忧古城那边的情况，但我还是决定现寻找高塔。果然，我非常顺利的经由|B|小树林||进入了|B|登拉克峡谷||。在峡谷中我发现了一处村落的遗迹，似乎已经荒废很多年了。进入到峡谷中心地带区域，我遇到了|G|科迪||，他就像是一只野蛮的猩猩，拦住了我的去路，并声称只能从他的尸体上过去。我只好照做，峡谷深处一直往里走，我进入到了一个山洞中。$|在漆黑的洞穴中一直走了半天时间，我发现自己竟然已经身处|B|玲珑峰||顶部。继续往里走，我吃惊地发现，我已经可以远远望见高塔了。就在这时，|G|米兰达||现身了，她说，他和|G|科迪||、|G|奥莱伊李||、|G|塞巴斯恰恩||曾经是“天启四骑士”。他们使用各种办法不让外人靠近|B|布萨特高塔||，而你可以到达这一关，已经是非常了不起了。|G|米兰达||并表示，我必须先找到三件道具，才可以进入高塔，否则也是打不开高塔的大门的。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>米兰达作为高塔前最后的守护者，要求我找到三件道具，才能进入高塔</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -229,14 +225,18 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>|击败了远古神兽之后，|G|塞尼斯||却消失了，他通过一个小孩告知了我|B|塔塔木村||是必经之路。然而，来到村子之后，我并没能够获得一些关于高塔有用的信息。于是，在进行了简单的补给之后，我只好继续往北走，进入|B|小树林||。|B|小树林||确实如其名，是一片很小的树林，但却是到达|B|登拉克峡谷||的必经之路。而后者是却被广阔的神秘森林所覆盖，很有可能隐藏了通往高塔的去路。|B|小树林||中我遇到了|G|塞巴斯恰恩||，在帮他解决了麻烦之后，他告诉我因为前几天的大雨，通往峡谷的道路已经被冲毁，现在只能绕道|B|村外田园||的小路过去。$|谢过他之后，我转到到达|B|村外田园||。但是这里的管家|G|奥莱伊李||却非常傲慢无礼，不管我如何解释，他不让我进入田园，并坚持这里没有通往高塔的道路。在我通过卡牌对决重伤|G|奥莱伊李||后，他终于说出了缘由。田园其实是一条通往|B|珀斯古城||的要道，而它的主人要他坚守于此，不让任何人进入。$|我终于意识到自己被欺骗了，就在我回去追问|G|塞巴斯恰恩||之时，他声称此时一群匪贼通过田园进入了古城，失去了|G|奥莱伊李||守护的田园，任何人都可以随意进出。</t>
+    <t>|通往峡谷的道路已然通畅，我非常顺利的经由|B|小树林||进入了|B|登拉克峡谷||。在峡谷中我发现了一处村落的遗迹，似乎已经荒废很多年了。进入到峡谷中心地带区域，我遇到了|G|科迪||，他就像是一只野蛮的猩猩，拦住了我的去路，并声称只能从他的尸体上过去。我只好照做，峡谷深处一直往里走，我进入到了一个山洞中。$|在漆黑的洞穴中一直走了半天时间，我发现自己竟然已经身处|B|玲珑峰||顶部。继续往里走，我吃惊地发现，我已经可以远远望见高塔了。就在这时，|G|米兰达||现身了，她说，他和|G|科迪||、|G|奥莱伊李||、|G|塞巴斯恰恩||曾经是“天启四骑士”。他们使用各种办法不让外人靠近|B|布萨特高塔||，而你可以到达这一关，已经是非常了不起了。|G|米兰达||并表示，我必须先找到三件道具，才可以进入高塔，否则也是打不开高塔的大门的。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>|击败了远古神兽之后，|G|塞尼斯||却消失了，他通过一个小孩告知了我|B|塔塔木村||是必经之路。然而，来到村子之后，我并没能够获得一些关于高塔有用的信息。于是，在进行了简单的补给之后，我只好继续往北走，进入|B|小树林||。|B|小树林||确实如其名，是一片很小的树林，但却是到达|B|登拉克峡谷||的必经之路。而后者是却被广阔的神秘森林所覆盖，很有可能隐藏了通往高塔的去路。|B|小树林||中我遇到了|G|塞巴斯恰恩||，在帮他解决了麻烦之后，他告诉我因为前几天的大雨，通往峡谷的道路已经被冲毁，现在只能绕道|B|村外田园||的小路过去。$|谢过他之后，我转到到达|B|村外田园||。但是这里的管家|G|奥莱伊李||却非常傲慢无礼，不管我如何解释，他不让我进入田园，并坚持这里没有通往高塔的道路。在我通过卡牌对决重伤|G|奥莱伊李||后，他终于说出了缘由。田园其实是一条通往|B|珀斯古城||的要道，而它的主人要他坚守于此，不让任何人进入。$|我终于意识到自己被欺骗了，当我回到|B|小树林||时，|G|塞巴斯恰恩||早已经离开了。</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -951,74 +951,6 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1054,14 +986,14 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="CAEACD"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1554,7 +1486,7 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="F7" t="s">
         <v>41</v>
@@ -1566,7 +1498,7 @@
         <v>42</v>
       </c>
       <c r="I7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.15">
@@ -1583,19 +1515,19 @@
         <v>5</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F8" t="s">
         <v>42</v>
       </c>
       <c r="G8" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" t="s">
         <v>49</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>50</v>
-      </c>
-      <c r="I8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.15">
@@ -1612,7 +1544,7 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.15">
@@ -1620,7 +1552,7 @@
         <v>12001001</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10">
         <v>2</v>

</xml_diff>

<commit_message>
fix the new dungeon info
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
+    <workbookView xWindow="600" yWindow="30" windowWidth="18135" windowHeight="8385"/>
   </bookViews>
   <sheets>
     <sheet name="Quest" sheetId="1" r:id="rId1"/>
@@ -225,18 +225,18 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>|通往峡谷的道路已然通畅，我非常顺利的经由|B|小树林||进入了|B|登拉克峡谷||。在峡谷中我发现了一处村落的遗迹，似乎已经荒废很多年了。进入到峡谷中心地带区域，我遇到了|G|科迪||，他就像是一只野蛮的猩猩，拦住了我的去路，并声称只能从他的尸体上过去。我只好照做，峡谷深处一直往里走，我进入到了一个山洞中。$|在漆黑的洞穴中一直走了半天时间，我发现自己竟然已经身处|B|玲珑峰||顶部。继续往里走，我吃惊地发现，我已经可以远远望见高塔了。就在这时，|G|米兰达||现身了，她说，他和|G|科迪||、|G|奥莱伊李||、|G|塞巴斯恰恩||曾经是“天启四骑士”。他们使用各种办法不让外人靠近|B|布萨特高塔||，而你可以到达这一关，已经是非常了不起了。|G|米兰达||并表示，我必须先找到三件道具，才可以进入高塔，否则也是打不开高塔的大门的。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>|击败了远古神兽之后，|G|塞尼斯||却消失了，他通过一个小孩告知了我|B|塔塔木村||是必经之路。然而，来到村子之后，我并没能够获得一些关于高塔有用的信息。于是，在进行了简单的补给之后，我只好继续往北走，进入|B|小树林||。|B|小树林||确实如其名，是一片很小的树林，但却是到达|B|登拉克峡谷||的必经之路。而后者是却被广阔的神秘森林所覆盖，很有可能隐藏了通往高塔的去路。|B|小树林||中我遇到了|G|塞巴斯恰恩||，在帮他解决了麻烦之后，他告诉我因为前几天的大雨，通往峡谷的道路已经被冲毁，现在只能绕道|B|村外田园||的小路过去。$|谢过他之后，我转到到达|B|村外田园||。但是这里的管家|G|奥莱伊李||却非常傲慢无礼，不管我如何解释，他不让我进入田园，并坚持这里没有通往高塔的道路。在我通过卡牌对决重伤|G|奥莱伊李||后，他终于说出了缘由。田园其实是一条通往|B|珀斯古城||的要道，而它的主人要他坚守于此，不让任何人进入。$|我终于意识到自己被欺骗了，当我回到|B|小树林||时，|G|塞巴斯恰恩||早已经离开了。</t>
+    <t>|击败了远古神兽之后，|G|塞尼斯||却消失了，他通过一个小孩告知了我|B|塔塔木村||是必经之路。然而，来到村子之后，我并没能够获得一些关于高塔有用的信息。于是，在进行了简单的补给之后，我只好继续往北走，进入|B|小树林||。|B|小树林||确实如其名，是一片很小的树林，但却是到达|B|登拉克峡谷||的必经之路。而后者是却被广阔的神秘森林所覆盖，很有可能隐藏了通往高塔的去路。|B|小树林||中我遇到了|G|塞巴斯恰恩||，在帮他解决了麻烦之后，他告诉我因为前几天的大雨，通往峡谷的道路已经被冲毁，现在只能绕道|B|村外田园||的小路过去。$|谢过他之后，我转而到达|B|村外田园||。但是这里的地头蛇|G|奥莱伊李||却非常傲慢无礼，不管我如何解释，他不让我进入田园，并坚持这里没有通往高塔的道路。在我通过卡牌对决重伤|G|奥莱伊李||后，他终于说出了缘由。田园其实是一条通往|B|珀斯古城||的要道，而它的主人要他坚守于此，不让任何人进入。$|我终于意识到自己被欺骗了，当我回到|B|小树林||时，|G|塞巴斯恰恩||早已经离开了。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>|通往峡谷的道路已然通畅，我非常顺利的经由|B|小树林||进入了|B|登拉克峡谷||。在峡谷中我发现了一处村落的遗迹，从中我发现了一些资料，记载着峡谷的历史和高塔的传说。进入到峡谷中心地带区域，我遇到了|G|科迪||，他就像是一只野蛮的猩猩，拦住了我的去路，并声称只能从他的尸体上过去。我只好照做，峡谷深处一直往里走，我进入到了一个山洞中。$|在漆黑的洞穴中一直走了半天时间，我发现自己竟然已经身处|B|玲珑峰||顶部。继续往里走，我吃惊地发现，我已经可以远远望见高塔了。就在这时，|G|米兰达||现身了，她说，他和|G|科迪||、|G|奥莱伊李||、|G|塞巴斯恰恩||曾经是“天启四骑士”。他们使用各种办法不让外人靠近|B|布萨特高塔||，而你可以到达这一关，已经是非常了不起了。|G|米兰达||并表示，我必须先找到三件道具，才可以进入高塔，否则也是打不开高塔的大门的。</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -986,7 +986,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1275,7 +1275,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1457,7 +1457,7 @@
         <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
         <v>35</v>
@@ -1486,7 +1486,7 @@
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F7" t="s">
         <v>41</v>

</xml_diff>

<commit_message>
remove the flag relative code
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,12 +18,45 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>张剑慧</author>
+  </authors>
+  <commentList>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>张剑慧:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+1 谈话
+2 清理场景
+99 特殊</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
   <si>
-    <t>铁匠和我说了很多关于我叔叔以前的故事，原来他曾经是一个十分厉害的卡片召唤师。</t>
-  </si>
-  <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -45,231 +78,234 @@
     <t>Descript</t>
   </si>
   <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>|在我成年礼的那天，一早我去拜访了|G|乔斯基叔叔||，他说为了准备了一份成年礼物。到了叔叔家，乔斯基给我讲述一个古老的故事。$|故事就发生在|B|塔塔木森林||的更北面。很久以前，有一位大陆上都非常有名的勇士离开|B|塔塔木村||，但是却误入了这片森林。勇士心中丝毫没有一点害怕，他的勇武使他充满了自信。就这样，在迷路的情况下，他一直向北走了两天，直到一座高塔挡住了他的去路。这其实就是传说中的|B|布萨特高塔||，一个通过历练就可以大大提升自己能力的地方。勇士当时并不知情，他当时毫不犹豫的进入了高塔，希望可以有所收获。。。从此，关于这位勇士就销声匿迹了，世界上再也没有关于他的传说。$$|乔斯基希望你可以找到|B|布萨特高塔||，并到其中锻炼自己。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>区域</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RegionId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>战斗地图</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>交互地图id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>交互场景位置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>金币奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>食物奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>精神奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>经验奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>奖励道具1</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>给予的祝福等级</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>解锁对象</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EnemyId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BattleMap</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SceneId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Position</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardGold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardMental</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardExp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardBlessLevel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RivalId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>奖励道具2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardFood</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardHealth</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardItem</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardDrop</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ename</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文名</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>怪物id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务npc</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NpcId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>名字</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>恰恰</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>离开地图重置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResetOnLeave</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>12000001|Start</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发场景事件</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>传说</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>|在我成年礼的那天，一早我去拜访了|G|乔斯基叔叔||，他说为了准备了一份成年礼物。到了叔叔家，乔斯基给我讲述一个古老的故事。$|故事就发生在|B|塔塔木森林||的更北面。很久以前，有一位大陆上都非常有名的勇士离开|B|塔塔木村||，但是却误入了这片森林。勇士心中丝毫没有一点害怕，他的勇武使他充满了自信。就这样，在迷路的情况下，他一直向北走了两天，直到一座高塔挡住了他的去路。这其实就是传说中的|B|布萨特高塔||，一个通过历练就可以大大提升自己能力的地方。勇士当时并不知情，他当时毫不犹豫的进入了高塔，希望可以有所收获。。。从此，关于这位勇士就销声匿迹了，世界上再也没有关于他的传说。$$|乔斯基希望你可以找到|B|布萨特高塔||，并到其中锻炼自己。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>欺骗</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>四骑士</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>钥匙</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>黑暗之门</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>神兽穷奇</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>|通过三把钥匙，我打开了高塔的大门，一切的谜题感觉就要在今天解开了。那我传说中的的勇士在塔内究竟找到了什么？高塔第一层都是一些关于塔历史的壁画，似乎没有什么奇怪的东西。找到阶梯后，我就进入到了第二层，这里充满了各种机关，并且从机关的类型看来，年代并不是非常久远。我开始怀疑这个塔从何而来，这里并不像一个古代文明的古迹。奇怪的是，越是接近塔顶，这里黑暗的力量就越强大。终于，我来到了塔顶，在这里发现了一扇异世界的传送门，而所有黑暗力量的怪物都是由此而来。再消灭了从门内出现的一批怪物后，我赶紧破坏掉了传送门。一切都结束了吗？</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>海滩</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>|击败了远古神兽之后，|G|塞尼斯||却消失了，他通过一个小孩告知了我|B|塔塔木村||是必经之路。然而，来到村子之后，我并没能够获得一些关于高塔有用的信息。于是，在进行了简单的补给之后，我只好继续往北走，进入|B|小树林||。|B|小树林||确实如其名，是一片很小的树林，但却是到达|B|登拉克峡谷||的必经之路。而后者是却被广阔的神秘森林所覆盖，很有可能隐藏了通往高塔的去路。|B|小树林||中我遇到了|G|塞巴斯恰恩||，在帮他解决了麻烦之后，他告诉我因为前几天的大雨，通往峡谷的道路已经被冲毁，现在只能绕道|B|村外田园||的小路过去。$|谢过他之后，我转而到达|B|村外田园||。但是这里的地头蛇|G|奥莱伊李||却非常傲慢无礼，不管我如何解释，他不让我进入田园，并坚持这里没有通往高塔的道路。在我通过卡牌对决重伤|G|奥莱伊李||后，他终于说出了缘由。田园其实是一条通往|B|珀斯古城||的要道，而它的主人要他坚守于此，不让任何人进入。$|我终于意识到自己被欺骗了，当我回到|B|小树林||时，|G|塞巴斯恰恩||早已经离开了。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>|让我非常吃惊的是，|G|米兰达||告诉我那三件道具其实是三把钥匙。|Y|智慧钥匙||、|Y|力量钥匙||、|Y|勇气钥匙||，这三把钥匙拼接在一起开启|B|布萨特高塔||的大门。在|G|米兰达||的帮助下，我先后获得了|Y|智慧钥匙||、|Y|力量钥匙||。但是|Y|勇气钥匙||却被存放在|B|珀斯古城||的最深处。看来我还是必须去一趟古城，去找寻这最后一把钥匙。$|在古城门口，我遇到了|G|威阿伊丁||，他要求所有人都对他施已王室的敬礼。他说他是这片王城的国王，但是战乱毁了这里，仅仅留下一片废墟。但是，我可以感觉到，他的神志并不是很正常，还是不要和他多做纠缠为好。$|古城内完全是一个黑暗的世界，这里的亡灵生物非常多，并且力量非常强大。通过层层的阻拦，我终于到达了最深处，并找到了传说中的|Y|勇气钥匙||。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>|通往峡谷的道路已然通畅，我非常顺利的经由|B|小树林||进入了|B|登拉克峡谷||。在峡谷中我发现了一处村落的遗迹，从中我发现了一些资料，记载着峡谷的历史和高塔的传说。进入到峡谷中心地带区域，我遇到了|G|科迪||，他就像是一只野蛮的猩猩，拦住了我的去路，并声称只能从他的尸体上过去。我只好照做，峡谷深处一直往里走，我进入到了一个山洞中。$|在漆黑的洞穴中一直走了半天时间，我发现自己竟然已经身处|B|玲珑峰||顶部。继续往里走，我吃惊地发现，我已经可以远远望见高塔了。就在这时，|G|米兰达||现身了，她说，他和|G|科迪||、|G|奥莱伊李||、|G|塞巴斯恰恩||曾经是“天启四骑士”。他们使用各种办法不让外人靠近|B|布萨特高塔||，而你可以到达这一关，已经是非常了不起了。|G|米兰达||并表示，我必须先找到三件道具，才可以进入高塔，否则也是打不开高塔的大门的。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>区域</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RegionId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>战斗地图</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>交互地图id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>交互场景位置</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>金币奖励系数</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>食物奖励系数</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>精神奖励系数</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>经验奖励系数</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>奖励道具1</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>给予的祝福等级</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>解锁对象</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>EnemyId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BattleMap</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SceneId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Position</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardGold</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardMental</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardExp</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardBlessLevel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RivalId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>生命奖励系数</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>奖励道具2</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardFood</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardHealth</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardItem</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardDrop</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ename</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>英文名</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>|就这样，我离开了自己的家，开始远行，寻找|B|布萨特高塔||。这个地方真的存在吗，或是如果存在，我真的能够找到吗，我完全没有把握。我决定先到达|B|塔塔木村||，那里说不定会有人可以给我一些信息。$B|昏暗密林||到往|B|塔塔木村||的必经之路。我对这片密林已经非常熟悉，从小时候就时常和叔叔一同在林间捕猎。虽然，林子中的狼偶尔会给我们带来一些麻烦。这次，我在林间偶然遇到了|G|塞尼斯||，他的右眼非常像龙的眼睛，并自称具有和龙沟通的能力。他说，经过几天的追踪，他发现了远古神兽|R|穷奇||的踪迹，并提出如果能够战胜他，就可以和他一同进入|B|密林深处|对决神兽。$|对决中，我利用法术渡过了前期的猛攻，后期利用|P|作战傀儡||加上强化法术，一波流带走对手。我的能力完全超出了|G|塞尼斯||的预想，他也同意了带我一起进入密林。$|这片森林处处充满着诡异的气氛，来回几次，我们发现自己只是在原地打转。偶然间，我们发现了森林的秘密，原来只有按照一定的顺序才能走出这个迷宫。而在迷宫尽头，我们找到了|R|穷奇||，一场大战看来已经不可避免。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>怪物id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>任务npc</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NpcId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>名字</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>序列</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>任务类型</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
+    <t>SceneQuestId2</t>
+  </si>
+  <si>
+    <t>清理农场</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectjob</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiaqia</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>aolai</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -277,7 +313,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -472,6 +508,19 @@
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="39">
@@ -935,7 +984,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -964,6 +1013,9 @@
       <alignment vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1011,7 +1063,27 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="5">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1031,13 +1103,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1052,12 +1117,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:T10" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A3:T10"/>
-  <sortState ref="A4:AE52">
-    <sortCondition ref="A3:A52"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:V6" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="A3:V6"/>
+  <sortState ref="A4:AG46">
+    <sortCondition ref="A3:A46"/>
   </sortState>
-  <tableColumns count="20">
+  <tableColumns count="22">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="19" name="Ename"/>
@@ -1065,6 +1130,8 @@
     <tableColumn id="13" name="Descript"/>
     <tableColumn id="20" name="NpcId"/>
     <tableColumn id="21" name="Type"/>
+    <tableColumn id="9" name="ResetOnLeave" dataDxfId="3"/>
+    <tableColumn id="23" name="SceneQuestId2" dataDxfId="2"/>
     <tableColumn id="5" name="EnemyId"/>
     <tableColumn id="6" name="BattleMap"/>
     <tableColumn id="7" name="SceneId"/>
@@ -1403,11 +1470,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1415,305 +1482,308 @@
     <col min="1" max="1" width="8.75" customWidth="1"/>
     <col min="4" max="4" width="6.5" customWidth="1"/>
     <col min="5" max="5" width="69.5" customWidth="1"/>
-    <col min="6" max="7" width="7.375" customWidth="1"/>
-    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.125" customWidth="1"/>
+    <col min="7" max="8" width="7.375" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="22" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:22" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="V1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="J3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
         <v>61</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q1" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="R1" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>42120001</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10"/>
+      <c r="N4">
+        <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>12000002</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>51</v>
+      </c>
+      <c r="C5" t="s">
+        <v>62</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
-      <c r="E5" t="s">
-        <v>55</v>
+      <c r="F5">
+        <v>42120003</v>
+      </c>
+      <c r="G5">
+        <v>99</v>
+      </c>
+      <c r="H5" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5">
+        <v>42120004</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>12000003</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>63</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>12000004</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>12000005</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A9">
-        <v>12000006</v>
-      </c>
-      <c r="B9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <v>12001001</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10">
+      <c r="F6">
+        <v>42120005</v>
+      </c>
+      <c r="G6">
         <v>2</v>
       </c>
-      <c r="E10" t="s">
-        <v>0</v>
-      </c>
+      <c r="H6" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="A4:L10">
-    <cfRule type="containsBlanks" dxfId="1" priority="1">
+  <conditionalFormatting sqref="J4:V6 A4:H6">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(A4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I4:I6">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(I4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
basically finish the quest form
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
     <author>张剑慧</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="I1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -306,6 +306,26 @@
   </si>
   <si>
     <t>aolai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1063,7 +1083,35 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1117,21 +1165,23 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:V6" totalsRowShown="0" headerRowDxfId="4">
-  <autoFilter ref="A3:V6"/>
-  <sortState ref="A4:AG46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:X12" totalsRowShown="0" headerRowDxfId="8">
+  <autoFilter ref="A3:X12"/>
+  <sortState ref="A4:AI46">
     <sortCondition ref="A3:A46"/>
   </sortState>
-  <tableColumns count="22">
+  <tableColumns count="24">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="19" name="Ename"/>
     <tableColumn id="4" name="RegionId"/>
+    <tableColumn id="22" name="X"/>
+    <tableColumn id="24" name="Y"/>
     <tableColumn id="13" name="Descript"/>
     <tableColumn id="20" name="NpcId"/>
     <tableColumn id="21" name="Type"/>
-    <tableColumn id="9" name="ResetOnLeave" dataDxfId="3"/>
-    <tableColumn id="23" name="SceneQuestId2" dataDxfId="2"/>
+    <tableColumn id="9" name="ResetOnLeave" dataDxfId="7"/>
+    <tableColumn id="23" name="SceneQuestId2" dataDxfId="6"/>
     <tableColumn id="5" name="EnemyId"/>
     <tableColumn id="6" name="BattleMap"/>
     <tableColumn id="7" name="SceneId"/>
@@ -1471,25 +1521,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.75" customWidth="1"/>
-    <col min="4" max="4" width="6.5" customWidth="1"/>
-    <col min="5" max="5" width="69.5" customWidth="1"/>
-    <col min="6" max="6" width="9.125" customWidth="1"/>
-    <col min="7" max="8" width="7.375" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="22" width="7.5" customWidth="1"/>
+    <col min="4" max="6" width="6.5" customWidth="1"/>
+    <col min="7" max="7" width="69.5" customWidth="1"/>
+    <col min="8" max="8" width="9.125" customWidth="1"/>
+    <col min="9" max="10" width="7.375" customWidth="1"/>
+    <col min="11" max="11" width="9" customWidth="1"/>
+    <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="24" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:24" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>47</v>
       </c>
@@ -1503,61 +1553,67 @@
         <v>8</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1571,40 +1627,40 @@
         <v>6</v>
       </c>
       <c r="E2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="H2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>21</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>20</v>
       </c>
       <c r="M2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>0</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>0</v>
@@ -1613,19 +1669,25 @@
         <v>0</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="T2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="U2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="V2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="W2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" s="6" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1639,61 +1701,67 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="I3" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="J3" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="K3" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="L3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="7" t="s">
+      <c r="O3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -1706,21 +1774,27 @@
       <c r="D4">
         <v>1</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>7</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>42120001</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>1</v>
       </c>
-      <c r="H4" s="10"/>
-      <c r="N4">
+      <c r="J4" s="10"/>
+      <c r="P4">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>12000002</v>
       </c>
@@ -1733,20 +1807,26 @@
       <c r="D5">
         <v>1</v>
       </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
       <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="H5">
         <v>42120003</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>99</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="J5" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>42120004</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>12000003</v>
       </c>
@@ -1759,24 +1839,144 @@
       <c r="D6">
         <v>1</v>
       </c>
+      <c r="E6">
+        <v>6</v>
+      </c>
       <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="H6">
         <v>42120005</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>2</v>
       </c>
-      <c r="H6" s="10"/>
+      <c r="J6" s="10"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>12000004</v>
+      </c>
+      <c r="B7">
+        <v>111</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>12000005</v>
+      </c>
+      <c r="B8">
+        <v>111</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>12000006</v>
+      </c>
+      <c r="B9">
+        <v>111</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>11</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>12000007</v>
+      </c>
+      <c r="B10">
+        <v>111</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>11</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>12000008</v>
+      </c>
+      <c r="B11">
+        <v>111</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
+      <c r="A12">
+        <v>12000009</v>
+      </c>
+      <c r="B12">
+        <v>111</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="J4:V6 A4:H6">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+  <conditionalFormatting sqref="L4:X12 A4:J12">
+    <cfRule type="containsBlanks" dxfId="5" priority="2">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I6">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(I4))=0</formula>
+  <conditionalFormatting sqref="K4:K12">
+    <cfRule type="containsBlanks" dxfId="4" priority="1">
+      <formula>LEN(TRIM(K4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
implement the basic task system
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -290,9 +290,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>SceneQuestId2</t>
-  </si>
-  <si>
     <t>清理农场</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -326,6 +323,10 @@
   </si>
   <si>
     <t>Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SceneQuestId</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1083,49 +1084,7 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1151,6 +1110,20 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1165,7 +1138,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:X12" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:X12" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A3:X12"/>
   <sortState ref="A4:AI46">
     <sortCondition ref="A3:A46"/>
@@ -1180,8 +1153,8 @@
     <tableColumn id="13" name="Descript"/>
     <tableColumn id="20" name="NpcId"/>
     <tableColumn id="21" name="Type"/>
-    <tableColumn id="9" name="ResetOnLeave" dataDxfId="7"/>
-    <tableColumn id="23" name="SceneQuestId2" dataDxfId="6"/>
+    <tableColumn id="9" name="ResetOnLeave" dataDxfId="1"/>
+    <tableColumn id="23" name="SceneQuestId" dataDxfId="0"/>
     <tableColumn id="5" name="EnemyId"/>
     <tableColumn id="6" name="BattleMap"/>
     <tableColumn id="7" name="SceneId"/>
@@ -1524,7 +1497,7 @@
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1553,10 +1526,10 @@
         <v>8</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>64</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>65</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>2</v>
@@ -1627,10 +1600,10 @@
         <v>6</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G2" s="9" t="s">
         <v>1</v>
@@ -1701,10 +1674,10 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>5</v>
@@ -1719,7 +1692,7 @@
         <v>54</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>23</v>
@@ -1769,7 +1742,7 @@
         <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -1789,7 +1762,12 @@
       <c r="I4">
         <v>1</v>
       </c>
-      <c r="J4" s="10"/>
+      <c r="J4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4">
+        <v>42120017</v>
+      </c>
       <c r="P4">
         <v>50</v>
       </c>
@@ -1802,7 +1780,7 @@
         <v>51</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5">
         <v>1</v>
@@ -1831,10 +1809,10 @@
         <v>12000003</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -1970,12 +1948,12 @@
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <conditionalFormatting sqref="L4:X12 A4:J12">
-    <cfRule type="containsBlanks" dxfId="5" priority="2">
+    <cfRule type="containsBlanks" dxfId="4" priority="2">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:K12">
-    <cfRule type="containsBlanks" dxfId="4" priority="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(K4))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add some quest mechanical
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -24,7 +24,7 @@
     <author>张剑慧</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -98,14 +98,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>交互地图id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>交互场景位置</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>金币奖励系数</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -142,51 +134,79 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>EnemyId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BattleMap</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardGold</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardMental</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardExp</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardBlessLevel</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RivalId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>生命奖励系数</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>奖励道具2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>EnemyId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BattleMap</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SceneId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Position</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardGold</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardMental</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardExp</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardBlessLevel</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RivalId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>生命奖励系数</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>奖励道具2</t>
+    <t>RewardFood</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardHealth</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardItem</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardDrop</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ename</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文名</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>怪物id</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务npc</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -194,39 +214,55 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>RewardFood</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardHealth</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardItem</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardDrop</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ename</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>英文名</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>怪物id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>任务npc</t>
+    <t>NpcId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>名字</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>恰恰</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>离开地图重置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResetOnLeave</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>12000001|Start</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发场景事件</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -234,55 +270,27 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>NpcId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>名字</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>序列</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>任务类型</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>开始</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>恰恰</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>离开地图重置</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ResetOnLeave</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>12000001|Start</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>触发场景事件</t>
+    <t>清理农场</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectjob</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiaqia</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>aolai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示y</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -290,27 +298,50 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>清理农场</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>selectjob</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>qiaqia</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>aolai</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>显示x</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>显示y</t>
+    <t>X</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SceneQuestId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>影响sq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>采集罂粟</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pickpoppy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>questpickpoppy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield</t>
+  </si>
+  <si>
+    <t>交互的脚本</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestScript</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>前置</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -318,15 +349,7 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>X</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SceneQuestId</t>
+    <t>Former</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1084,7 +1107,28 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1110,20 +1154,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1138,27 +1168,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:X12" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A3:X12"/>
-  <sortState ref="A4:AI46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Y12" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A3:Y12"/>
+  <sortState ref="A4:AJ46">
     <sortCondition ref="A3:A46"/>
   </sortState>
-  <tableColumns count="24">
+  <tableColumns count="25">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="19" name="Ename"/>
+    <tableColumn id="25" name="Former"/>
     <tableColumn id="4" name="RegionId"/>
     <tableColumn id="22" name="X"/>
     <tableColumn id="24" name="Y"/>
     <tableColumn id="13" name="Descript"/>
     <tableColumn id="20" name="NpcId"/>
     <tableColumn id="21" name="Type"/>
-    <tableColumn id="9" name="ResetOnLeave" dataDxfId="1"/>
-    <tableColumn id="23" name="SceneQuestId" dataDxfId="0"/>
+    <tableColumn id="9" name="ResetOnLeave" dataDxfId="4"/>
+    <tableColumn id="23" name="SceneQuestId" dataDxfId="3"/>
     <tableColumn id="5" name="EnemyId"/>
     <tableColumn id="6" name="BattleMap"/>
-    <tableColumn id="7" name="SceneId"/>
-    <tableColumn id="8" name="Position"/>
+    <tableColumn id="7" name="SceneQuest"/>
+    <tableColumn id="8" name="QuestScript"/>
     <tableColumn id="10" name="RewardGold"/>
     <tableColumn id="3" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
@@ -1494,99 +1525,103 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X12"/>
+  <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.75" customWidth="1"/>
-    <col min="4" max="6" width="6.5" customWidth="1"/>
-    <col min="7" max="7" width="69.5" customWidth="1"/>
-    <col min="8" max="8" width="9.125" customWidth="1"/>
-    <col min="9" max="10" width="7.375" customWidth="1"/>
-    <col min="11" max="11" width="9" customWidth="1"/>
-    <col min="13" max="13" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="24" width="7.5" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="6.5" customWidth="1"/>
+    <col min="8" max="8" width="69.5" customWidth="1"/>
+    <col min="9" max="9" width="9.125" customWidth="1"/>
+    <col min="10" max="11" width="7.375" customWidth="1"/>
+    <col min="12" max="12" width="9" customWidth="1"/>
+    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="25" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:25" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F1" s="8" t="s">
+      <c r="L1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="R1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="S1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="S1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="W1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1594,49 +1629,49 @@
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>65</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="M2" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="R2" s="6" t="s">
         <v>0</v>
@@ -1648,19 +1683,22 @@
         <v>0</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>34</v>
+        <v>0</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="W2" s="6" t="s">
         <v>0</v>
       </c>
       <c r="X2" s="6" t="s">
-        <v>34</v>
+        <v>0</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1668,84 +1706,84 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s">
         <v>45</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="L3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="M3" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="N3" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="O3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
+      <c r="C4" t="s">
         <v>55</v>
-      </c>
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1753,208 +1791,231 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
         <v>7</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>42120001</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>1</v>
       </c>
-      <c r="J4" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="K4">
+      <c r="K4" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4">
         <v>42120017</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>12000002</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5">
+        <v>56</v>
+      </c>
+      <c r="E5">
         <v>1</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
       </c>
       <c r="F5">
         <v>3</v>
       </c>
-      <c r="H5">
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="I5">
         <v>42120003</v>
       </c>
-      <c r="I5">
-        <v>99</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="K5">
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="L5">
         <v>42120004</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>12000003</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D6">
+        <v>57</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>6</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>2</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>42120005</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>2</v>
       </c>
-      <c r="J6" s="10"/>
+      <c r="K6" s="10"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>12000004</v>
       </c>
-      <c r="B7">
-        <v>111</v>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
       </c>
       <c r="D7">
+        <v>12000001</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="E7">
-        <v>8</v>
-      </c>
       <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
         <v>2</v>
       </c>
-      <c r="J7" s="10"/>
+      <c r="I7">
+        <v>42120001</v>
+      </c>
       <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="O7" t="s">
+        <v>69</v>
+      </c>
+      <c r="P7" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>12000005</v>
       </c>
       <c r="B8">
         <v>111</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>1</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>10</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>5</v>
       </c>
-      <c r="J8" s="10"/>
       <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>12000006</v>
       </c>
       <c r="B9">
         <v>111</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>11</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>4</v>
       </c>
-      <c r="J9" s="10"/>
       <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>12000007</v>
       </c>
       <c r="B10">
         <v>111</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>1</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>11</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>2</v>
       </c>
-      <c r="J10" s="10"/>
       <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>12000008</v>
       </c>
       <c r="B11">
         <v>111</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>9</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>2</v>
       </c>
-      <c r="J11" s="10"/>
       <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>12000009</v>
       </c>
       <c r="B12">
         <v>111</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>4</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>5</v>
       </c>
-      <c r="J12" s="10"/>
       <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="L4:X12 A4:J12">
-    <cfRule type="containsBlanks" dxfId="4" priority="2">
+  <conditionalFormatting sqref="M4:Y5 M6:N6 A4:K12 M7:Y12 P6:Y6">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4:K12">
-    <cfRule type="containsBlanks" dxfId="3" priority="1">
-      <formula>LEN(TRIM(K4))=0</formula>
+  <conditionalFormatting sqref="L4:L12">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(L4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O6">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(O6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
tip support rich text. fix a bug of text measure width bug
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -351,6 +351,9 @@
   <si>
     <t>Former</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|乔斯基||让我去找|G|瓦里斯||，并向他学习战斗的技巧，提升自己。</t>
   </si>
 </sst>
 </file>
@@ -1528,7 +1531,7 @@
   <dimension ref="A1:Y12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1893,6 +1896,9 @@
       </c>
       <c r="G7">
         <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>75</v>
       </c>
       <c r="I7">
         <v>42120001</v>

</xml_diff>

<commit_message>
support new quest type
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,44 +18,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>张剑慧</author>
-  </authors>
-  <commentList>
-    <comment ref="J1" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t>张剑慧:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="宋体"/>
-            <charset val="134"/>
-          </rPr>
-          <t xml:space="preserve">
-1 谈话
-2 清理场景
-99 特殊</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -82,10 +46,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>|在我成年礼的那天，一早我去拜访了|G|乔斯基叔叔||，他说为了准备了一份成年礼物。到了叔叔家，乔斯基给我讲述一个古老的故事。$|故事就发生在|B|塔塔木森林||的更北面。很久以前，有一位大陆上都非常有名的勇士离开|B|塔塔木村||，但是却误入了这片森林。勇士心中丝毫没有一点害怕，他的勇武使他充满了自信。就这样，在迷路的情况下，他一直向北走了两天，直到一座高塔挡住了他的去路。这其实就是传说中的|B|布萨特高塔||，一个通过历练就可以大大提升自己能力的地方。勇士当时并不知情，他当时毫不犹豫的进入了高塔，希望可以有所收获。。。从此，关于这位勇士就销声匿迹了，世界上再也没有关于他的传说。$$|乔斯基希望你可以找到|B|布萨特高塔||，并到其中锻炼自己。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>区域</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -94,10 +54,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>战斗地图</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>金币奖励系数</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -134,14 +90,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>EnemyId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>BattleMap</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>RewardGold</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -202,10 +150,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>怪物id</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>任务npc</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -254,15 +198,31 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>12000001|Start</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>true</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>触发场景事件</t>
+    <t>清理农场</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectjob</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiaqia</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>aolai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示y</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -270,27 +230,42 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>清理农场</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>selectjob</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>qiaqia</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>aolai</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>显示x</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>显示y</t>
+    <t>X</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>影响sq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>采集罂粟</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pickpoppy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>questpickpoppy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield</t>
+  </si>
+  <si>
+    <t>交互的脚本</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestScript</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>前置</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -298,50 +273,31 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>X</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SceneQuestId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>影响sq</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SceneQuest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>采集罂粟</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>pickpoppy</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>questpickpoppy</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>poppyfield</t>
-  </si>
-  <si>
-    <t>交互的脚本</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QuestScript</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>前置</t>
+    <t>Former</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|乔斯基||让你去找|G|瓦里斯||，并向他学习战斗的技巧，提升自己。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|乔斯基||需要一些罂粟花苗，让你寻找收集一些。应该可以从|O|罂粟花田||中找到。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>狼群的威胁</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfflow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞尼斯||希望你帮助他，进入附近的|O|狼穴|并消灭狼群，如果失败了，你可以尝试反复进出本地图重试。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>进度变化</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -349,18 +305,65 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Former</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|乔斯基||让我去找|G|瓦里斯||，并向他学习战斗的技巧，提升自己。</t>
+    <t>ProgressAdd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发sq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcwalisi</t>
+  </si>
+  <si>
+    <t>npcqiaqia</t>
+  </si>
+  <si>
+    <t>TriggerSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成sq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SuccessSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>变化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>成功</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -556,21 +559,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="39">
+  <fills count="46">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -783,6 +773,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1031,7 +1063,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1063,6 +1095,33 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1110,7 +1169,21 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1171,10 +1244,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Y12" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A3:Y12"/>
-  <sortState ref="A4:AJ46">
-    <sortCondition ref="A3:A46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Y13" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="A3:Y13"/>
+  <sortState ref="A4:Y13">
+    <sortCondition ref="A3:A13"/>
   </sortState>
   <tableColumns count="25">
     <tableColumn id="1" name="Id"/>
@@ -1187,12 +1260,12 @@
     <tableColumn id="13" name="Descript"/>
     <tableColumn id="20" name="NpcId"/>
     <tableColumn id="21" name="Type"/>
-    <tableColumn id="9" name="ResetOnLeave" dataDxfId="4"/>
-    <tableColumn id="23" name="SceneQuestId" dataDxfId="3"/>
-    <tableColumn id="5" name="EnemyId"/>
-    <tableColumn id="6" name="BattleMap"/>
-    <tableColumn id="7" name="SceneQuest"/>
+    <tableColumn id="9" name="ResetOnLeave" dataDxfId="6"/>
+    <tableColumn id="23" name="TriggerSceneQuest" dataDxfId="5"/>
+    <tableColumn id="7" name="CheckSceneQuest"/>
+    <tableColumn id="27" name="ProgressAdd"/>
     <tableColumn id="8" name="QuestScript"/>
+    <tableColumn id="28" name="SuccessSceneQuest"/>
     <tableColumn id="10" name="RewardGold"/>
     <tableColumn id="3" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
@@ -1527,11 +1600,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1543,85 +1616,84 @@
     <col min="9" max="9" width="9.125" customWidth="1"/>
     <col min="10" max="11" width="7.375" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="14" max="14" width="9.5" bestFit="1" customWidth="1"/>
     <col min="17" max="25" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="N1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="M1" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q1" s="4" t="s">
+      <c r="S1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="T1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.15">
@@ -1632,49 +1704,49 @@
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>0</v>
+        <v>82</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="L2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>19</v>
+        <v>1</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="O2" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>79</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="R2" s="6" t="s">
         <v>0</v>
@@ -1689,7 +1761,7 @@
         <v>0</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="W2" s="6" t="s">
         <v>0</v>
@@ -1698,7 +1770,7 @@
         <v>0</v>
       </c>
       <c r="Y2" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.15">
@@ -1709,84 +1781,84 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="J3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="K3" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="L3" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="M3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="P3" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="V3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="X3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="X3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>50</v>
+      <c r="A4">
+        <v>12000001</v>
       </c>
       <c r="B4" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1798,19 +1870,19 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>7</v>
+        <v>65</v>
       </c>
       <c r="I4">
         <v>42120001</v>
       </c>
-      <c r="J4">
-        <v>1</v>
+      <c r="J4" s="17" t="s">
+        <v>83</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4">
-        <v>42120017</v>
+        <v>45</v>
+      </c>
+      <c r="L4" t="s">
+        <v>75</v>
       </c>
       <c r="Q4">
         <v>50</v>
@@ -1821,10 +1893,13 @@
         <v>12000002</v>
       </c>
       <c r="B5" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>57</v>
+      </c>
+      <c r="D5">
+        <v>12000001</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -1833,19 +1908,30 @@
         <v>3</v>
       </c>
       <c r="G5">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
+        <v>66</v>
       </c>
       <c r="I5">
-        <v>42120003</v>
-      </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="L5">
-        <v>42120004</v>
+        <v>42120001</v>
+      </c>
+      <c r="J5" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5">
+        <v>10</v>
+      </c>
+      <c r="O5" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q5">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.15">
@@ -1853,83 +1939,95 @@
         <v>12000003</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>67</v>
       </c>
       <c r="C6" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
       <c r="F6">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G6">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>69</v>
       </c>
       <c r="I6">
-        <v>42120005</v>
-      </c>
-      <c r="J6">
-        <v>2</v>
+        <v>42120002</v>
+      </c>
+      <c r="J6" s="19" t="s">
+        <v>85</v>
       </c>
       <c r="K6" s="10"/>
+      <c r="N6">
+        <v>5</v>
+      </c>
+      <c r="P6" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>12000004</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7">
-        <v>12000001</v>
+        <v>48</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>2</v>
-      </c>
-      <c r="H7" t="s">
-        <v>75</v>
+        <v>3</v>
       </c>
       <c r="I7">
-        <v>42120001</v>
-      </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="O7" t="s">
-        <v>69</v>
-      </c>
-      <c r="P7" t="s">
-        <v>68</v>
+        <v>42120003</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="K7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>12000005</v>
       </c>
-      <c r="B8">
-        <v>111</v>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>49</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G8">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="I8">
+        <v>42120005</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
       </c>
       <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A9">
@@ -1942,10 +2040,10 @@
         <v>1</v>
       </c>
       <c r="F9">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="K9" s="10"/>
       <c r="L9" s="10"/>
@@ -1964,7 +2062,7 @@
         <v>11</v>
       </c>
       <c r="G10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
@@ -1980,7 +2078,7 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G11">
         <v>2</v>
@@ -1999,36 +2097,64 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="G12">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
     </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+      <c r="A13">
+        <v>12000010</v>
+      </c>
+      <c r="B13">
+        <v>111</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>4</v>
+      </c>
+      <c r="G13">
+        <v>5</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="M4:Y5 M6:N6 A4:K12 M7:Y12 P6:Y6">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+  <conditionalFormatting sqref="A7 A9 A11 A13 O6:Y7 M8:Y13 A4:Y5 B7:L13">
+    <cfRule type="containsBlanks" dxfId="4" priority="6">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L4:L12">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
-      <formula>LEN(TRIM(L4))=0</formula>
+  <conditionalFormatting sqref="M7:N7">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(M7))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O6">
+  <conditionalFormatting sqref="A6:G6 A8 A10 A12 I6:L6">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(A6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M6:N6">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(M6))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H6">
     <cfRule type="containsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(O6))=0</formula>
+      <formula>LEN(TRIM(H6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add the find kid quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="Quest" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -293,10 +293,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>G|塞尼斯||希望你帮助他，进入附近的|O|狼穴|并消灭狼群，如果失败了，你可以尝试反复进出本地图重试。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>进度变化</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -370,11 +366,30 @@
     <t>bossqiongqi</t>
   </si>
   <si>
-    <t>G|塞尼斯||告诉你，再附近的森林深处，有一只神兽|O|穷奇|，如果你可以找到并击败他，会得到丰厚的回报。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>rwqiongqi</t>
+  </si>
+  <si>
+    <t>G|玛莎||告诉你，他的孩子，前几天走失了。如果你碰到了这个孩子，一定要记得把他带回来</t>
+  </si>
+  <si>
+    <t>对话</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>走失的孩子</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lossboy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞尼斯||希望你帮助他，进入附近的|O|狼穴||并消灭狼群，如果失败了，你可以尝试反复进出本地图重试。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞尼斯||告诉你，再附近的森林深处，有一只神兽|O|穷奇||，如果你可以找到并击败他，会得到丰厚的回报。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -578,7 +593,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="46">
+  <fills count="47">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -833,6 +848,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1081,7 +1102,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1140,6 +1161,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1642,8 +1666,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1693,19 +1717,19 @@
         <v>42</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M1" s="11" t="s">
         <v>55</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O1" s="11" t="s">
         <v>60</v>
       </c>
       <c r="P1" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q1" s="4" t="s">
         <v>9</v>
@@ -1764,7 +1788,7 @@
         <v>34</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>43</v>
@@ -1776,13 +1800,13 @@
         <v>17</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>17</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="Q2" s="6" t="s">
         <v>16</v>
@@ -1847,19 +1871,19 @@
         <v>44</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O3" s="13" t="s">
         <v>61</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q3" s="2" t="s">
         <v>18</v>
@@ -1915,13 +1939,13 @@
         <v>42120001</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>45</v>
       </c>
       <c r="L4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q4">
         <v>50</v>
@@ -1956,7 +1980,7 @@
         <v>42120001</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
@@ -1993,20 +2017,20 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>69</v>
+        <v>93</v>
       </c>
       <c r="I6">
         <v>42120002</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K6" s="10"/>
       <c r="N6">
         <v>5</v>
       </c>
       <c r="P6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:25" x14ac:dyDescent="0.15">
@@ -2014,10 +2038,10 @@
         <v>12000004</v>
       </c>
       <c r="B7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" t="s">
         <v>86</v>
-      </c>
-      <c r="C7" t="s">
-        <v>87</v>
       </c>
       <c r="D7">
         <v>12000003</v>
@@ -2032,13 +2056,13 @@
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="I7">
         <v>42120002</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
@@ -2046,7 +2070,7 @@
         <v>10</v>
       </c>
       <c r="P7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="Q7">
         <v>300</v>
@@ -2058,7 +2082,7 @@
         <v>300</v>
       </c>
       <c r="V7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.15">
@@ -2084,13 +2108,13 @@
         <v>42120003</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>45</v>
       </c>
       <c r="L8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.15">
@@ -2124,20 +2148,35 @@
       <c r="A10">
         <v>12000007</v>
       </c>
-      <c r="B10">
-        <v>111</v>
+      <c r="B10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="G10">
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I10">
+        <v>42120014</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>90</v>
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
+      <c r="Q10">
+        <v>100</v>
+      </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.15">
       <c r="A11">

</xml_diff>

<commit_message>
finish 2 quest and relative mechanical
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="102">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -194,136 +194,213 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>清理农场</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectjob</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiaqia</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>aolai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>影响sq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>采集罂粟</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pickpoppy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>questpickpoppy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield</t>
+  </si>
+  <si>
+    <t>交互的脚本</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestScript</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>前置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Former</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|乔斯基||让你去找|G|瓦里斯||，并向他学习战斗的技巧，提升自己。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|乔斯基||需要一些罂粟花苗，让你寻找收集一些。应该可以从|O|罂粟花田||中找到。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>狼群的威胁</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfflow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>进度变化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProgressAdd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发sq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcwalisi</t>
+  </si>
+  <si>
+    <t>npcqiaqia</t>
+  </si>
+  <si>
+    <t>TriggerSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成sq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SuccessSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>变化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>成功</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>穷奇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiongqi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossqiongqi</t>
+  </si>
+  <si>
+    <t>rwqiongqi</t>
+  </si>
+  <si>
+    <t>G|玛莎||告诉你，他的孩子，前几天走失了。如果你碰到了这个孩子，一定要记得把他带回来</t>
+  </si>
+  <si>
+    <t>对话</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>走失的孩子</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lossboy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞尼斯||希望你帮助他，进入附近的|O|狼穴||并消灭狼群，如果失败了，你可以尝试反复进出本地图重试。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞尼斯||告诉你，再附近的森林深处，有一只神兽|O|穷奇||，如果你可以找到并击败他，会得到丰厚的回报。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞巴斯恰恩||的宠物|G|恰恰||不见了，他希望你可以帮助他找回宠物。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|奥莱伊李||觉得目前的田野很不安全，希望你可以帮助他清理当前场景的所有特殊事件。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>ResetOnLeave</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>清理农场</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>selectjob</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>qiaqia</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>aolai</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>显示x</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>显示y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>影响sq</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>采集罂粟</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>pickpoppy</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>questpickpoppy</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>poppyfield</t>
-  </si>
-  <si>
-    <t>交互的脚本</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QuestScript</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>前置</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Former</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|乔斯基||让你去找|G|瓦里斯||，并向他学习战斗的技巧，提升自己。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|乔斯基||需要一些罂粟花苗，让你寻找收集一些。应该可以从|O|罂粟花田||中找到。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>狼群的威胁</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfflow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>进度变化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ProgressAdd</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>CheckSceneQuest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>触发sq</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npcwalisi</t>
-  </si>
-  <si>
-    <t>npcqiaqia</t>
-  </si>
-  <si>
-    <t>TriggerSceneQuest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成sq</t>
+    <t>事件触发</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -331,64 +408,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>SuccessSceneQuest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfnest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>触发</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>变化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>成功</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>穷奇</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>qiongqi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bossqiongqi</t>
-  </si>
-  <si>
-    <t>rwqiongqi</t>
-  </si>
-  <si>
-    <t>G|玛莎||告诉你，他的孩子，前几天走失了。如果你碰到了这个孩子，一定要记得把他带回来</t>
-  </si>
-  <si>
-    <t>对话</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>走失的孩子</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>lossboy</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|塞尼斯||希望你帮助他，进入附近的|O|狼穴||并消灭狼群，如果失败了，你可以尝试反复进出本地图重试。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|塞尼斯||告诉你，再附近的森林深处，有一只神兽|O|穷奇||，如果你可以找到并击败他，会得到丰厚的回报。</t>
+    <t>allopen</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedAction</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1102,7 +1130,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1164,6 +1192,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1212,31 +1246,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="11">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="2"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1293,6 +1302,31 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1307,12 +1341,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Y14" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A3:Y14"/>
-  <sortState ref="A4:Y14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:Z14" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="A3:Z14"/>
+  <sortState ref="A4:Z14">
     <sortCondition ref="A3:A14"/>
   </sortState>
-  <tableColumns count="25">
+  <tableColumns count="26">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="19" name="Ename"/>
@@ -1323,12 +1357,13 @@
     <tableColumn id="13" name="Descript"/>
     <tableColumn id="20" name="NpcId"/>
     <tableColumn id="21" name="Type"/>
-    <tableColumn id="9" name="ResetOnLeave" dataDxfId="1"/>
-    <tableColumn id="23" name="TriggerSceneQuest" dataDxfId="0"/>
+    <tableColumn id="9" name="ResetOnLeave" dataDxfId="9"/>
+    <tableColumn id="23" name="TriggerSceneQuest" dataDxfId="8"/>
     <tableColumn id="7" name="CheckSceneQuest"/>
     <tableColumn id="27" name="ProgressAdd"/>
     <tableColumn id="8" name="QuestScript"/>
     <tableColumn id="28" name="SuccessSceneQuest"/>
+    <tableColumn id="5" name="NeedAction"/>
     <tableColumn id="10" name="RewardGold"/>
     <tableColumn id="3" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
@@ -1664,7 +1699,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:Z14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
@@ -1679,10 +1714,10 @@
     <col min="9" max="9" width="9.125" customWidth="1"/>
     <col min="10" max="11" width="7.375" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="17" max="25" width="7.5" customWidth="1"/>
+    <col min="18" max="26" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:26" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
         <v>37</v>
       </c>
@@ -1693,16 +1728,16 @@
         <v>32</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>50</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>51</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>2</v>
@@ -1717,49 +1752,52 @@
         <v>42</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P1" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q1" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="R1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
@@ -1770,16 +1808,16 @@
         <v>30</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>1</v>
@@ -1788,7 +1826,7 @@
         <v>34</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>43</v>
@@ -1800,19 +1838,19 @@
         <v>17</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>17</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="R2" s="6" t="s">
         <v>16</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>0</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>0</v>
@@ -1824,19 +1862,22 @@
         <v>0</v>
       </c>
       <c r="V2" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="X2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="Y2" s="6" t="s">
+      <c r="Z2" s="6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1847,16 +1888,16 @@
         <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>5</v>
@@ -1868,52 +1909,55 @@
         <v>39</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>44</v>
+        <v>96</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O3" s="13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q3" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q3" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="R3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="S3" s="2" t="s">
+      <c r="T3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="U3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="V3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>12000001</v>
       </c>
@@ -1921,7 +1965,7 @@
         <v>40</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -1933,33 +1977,33 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I4">
         <v>42120001</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L4" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q4">
+        <v>73</v>
+      </c>
+      <c r="R4">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>12000002</v>
       </c>
       <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
         <v>56</v>
-      </c>
-      <c r="C5" t="s">
-        <v>57</v>
       </c>
       <c r="D5">
         <v>12000001</v>
@@ -1974,38 +2018,38 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I5">
         <v>42120001</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N5">
         <v>10</v>
       </c>
       <c r="O5" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q5">
+        <v>57</v>
+      </c>
+      <c r="R5">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>12000003</v>
       </c>
       <c r="B6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" t="s">
         <v>67</v>
-      </c>
-      <c r="C6" t="s">
-        <v>68</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2017,31 +2061,31 @@
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I6">
         <v>42120002</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K6" s="10"/>
       <c r="N6">
         <v>5</v>
       </c>
       <c r="P6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>12000004</v>
       </c>
       <c r="B7" t="s">
+        <v>84</v>
+      </c>
+      <c r="C7" t="s">
         <v>85</v>
-      </c>
-      <c r="C7" t="s">
-        <v>86</v>
       </c>
       <c r="D7">
         <v>12000003</v>
@@ -2056,13 +2100,13 @@
         <v>4</v>
       </c>
       <c r="H7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I7">
         <v>42120002</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
@@ -2070,22 +2114,22 @@
         <v>10</v>
       </c>
       <c r="P7" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q7">
-        <v>300</v>
-      </c>
-      <c r="S7">
+        <v>86</v>
+      </c>
+      <c r="R7">
         <v>300</v>
       </c>
       <c r="T7">
         <v>300</v>
       </c>
-      <c r="V7" t="s">
-        <v>88</v>
+      <c r="U7">
+        <v>300</v>
+      </c>
+      <c r="W7" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>12000005</v>
       </c>
@@ -2093,39 +2137,45 @@
         <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
       <c r="F8">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G8">
         <v>3</v>
       </c>
+      <c r="H8" t="s">
+        <v>94</v>
+      </c>
       <c r="I8">
         <v>42120003</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L8" t="s">
-        <v>75</v>
+        <v>74</v>
+      </c>
+      <c r="R8">
+        <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>12000006</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2136,49 +2186,60 @@
       <c r="G9">
         <v>2</v>
       </c>
+      <c r="H9" t="s">
+        <v>95</v>
+      </c>
       <c r="I9">
         <v>42120005</v>
       </c>
-      <c r="J9">
-        <v>2</v>
-      </c>
-      <c r="K9" s="10"/>
+      <c r="J9" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>99</v>
+      </c>
+      <c r="R9">
+        <v>100</v>
+      </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>12000007</v>
       </c>
       <c r="B10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
         <v>91</v>
-      </c>
-      <c r="C10" t="s">
-        <v>92</v>
       </c>
       <c r="E10">
         <v>1</v>
       </c>
       <c r="F10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G10">
         <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I10">
         <v>42120014</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
-      <c r="Q10">
+      <c r="R10">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>12000008</v>
       </c>
@@ -2197,7 +2258,7 @@
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>12000009</v>
       </c>
@@ -2216,7 +2277,7 @@
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>12000010</v>
       </c>
@@ -2235,7 +2296,7 @@
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>12000011</v>
       </c>
@@ -2256,43 +2317,43 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="M9:Y14 A4:Y5 B8:L14 O6:Y6 O8:Y8 A7:G7 A8 A10:A11 A13:A14 K7:Y7">
-    <cfRule type="containsBlanks" dxfId="10" priority="9">
+  <conditionalFormatting sqref="M9:Z14 A4:Z5 O6:Z6 O8:Z8 A7:G7 A8 A10:A11 A13:A14 K7:Z7 B8:L14">
+    <cfRule type="containsBlanks" dxfId="7" priority="9">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8:N8">
-    <cfRule type="containsBlanks" dxfId="9" priority="7">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
       <formula>LEN(TRIM(M8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:G6 I6:L6 A9 A12">
-    <cfRule type="containsBlanks" dxfId="8" priority="6">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
       <formula>LEN(TRIM(A6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6:N6">
-    <cfRule type="containsBlanks" dxfId="7" priority="5">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
       <formula>LEN(TRIM(M6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsBlanks" dxfId="6" priority="4">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
       <formula>LEN(TRIM(H6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="containsBlanks" dxfId="5" priority="3">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
       <formula>LEN(TRIM(J7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="containsBlanks" dxfId="4" priority="2">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
       <formula>LEN(TRIM(I7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="containsBlanks" dxfId="3" priority="1">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(H7))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
add one new quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -246,214 +246,232 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>poppyfield</t>
+  </si>
+  <si>
+    <t>交互的脚本</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestScript</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>前置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Former</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|乔斯基||让你去找|G|瓦里斯||，并向他学习战斗的技巧，提升自己。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|乔斯基||需要一些罂粟花苗，让你寻找收集一些。应该可以从|O|罂粟花田||中找到。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>狼群的威胁</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfflow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>进度变化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProgressAdd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发sq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcwalisi</t>
+  </si>
+  <si>
+    <t>npcqiaqia</t>
+  </si>
+  <si>
+    <t>TriggerSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成sq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SuccessSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>成功</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>穷奇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiongqi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossqiongqi</t>
+  </si>
+  <si>
+    <t>rwqiongqi</t>
+  </si>
+  <si>
+    <t>G|玛莎||告诉你，他的孩子，前几天走失了。如果你碰到了这个孩子，一定要记得把他带回来</t>
+  </si>
+  <si>
+    <t>对话</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>走失的孩子</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lossboy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞尼斯||希望你帮助他，进入附近的|O|狼穴||并消灭狼群，如果失败了，你可以尝试反复进出本地图重试。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞尼斯||告诉你，再附近的森林深处，有一只神兽|O|穷奇||，如果你可以找到并击败他，会得到丰厚的回报。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞巴斯恰恩||的宠物|G|恰恰||不见了，他希望你可以帮助他找回宠物。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|奥莱伊李||觉得目前的田野很不安全，希望你可以帮助他清理当前场景的所有特殊事件。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResetOnLeave</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件触发</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>allopen</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedAction</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RequireItem</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>种植课程</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>plant</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>增项</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zwwandou</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zzwandou</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|奥莱伊李||教了你种植植物的方法，||你需要到附近的田地里，种下|Y|豌豆种子||。并在收获后，把果实带交给他。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>questpickpoppy</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>poppyfield</t>
-  </si>
-  <si>
-    <t>交互的脚本</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QuestScript</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>前置</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Former</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|乔斯基||让你去找|G|瓦里斯||，并向他学习战斗的技巧，提升自己。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|乔斯基||需要一些罂粟花苗，让你寻找收集一些。应该可以从|O|罂粟花田||中找到。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>狼群的威胁</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfflow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>进度变化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ProgressAdd</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>CheckSceneQuest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>触发sq</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npcwalisi</t>
-  </si>
-  <si>
-    <t>npcqiaqia</t>
-  </si>
-  <si>
-    <t>TriggerSceneQuest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成sq</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SuccessSceneQuest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfnest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>触发</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>成功</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>穷奇</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>qiongqi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bossqiongqi</t>
-  </si>
-  <si>
-    <t>rwqiongqi</t>
-  </si>
-  <si>
-    <t>G|玛莎||告诉你，他的孩子，前几天走失了。如果你碰到了这个孩子，一定要记得把他带回来</t>
-  </si>
-  <si>
-    <t>对话</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>走失的孩子</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>lossboy</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|塞尼斯||希望你帮助他，进入附近的|O|狼穴||并消灭狼群，如果失败了，你可以尝试反复进出本地图重试。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|塞尼斯||告诉你，再附近的森林深处，有一只神兽|O|穷奇||，如果你可以找到并击败他，会得到丰厚的回报。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|塞巴斯恰恩||的宠物|G|恰恰||不见了，他希望你可以帮助他找回宠物。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|奥莱伊李||觉得目前的田野很不安全，希望你可以帮助他清理当前场景的所有特殊事件。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ResetOnLeave</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>事件触发</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>allopen</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>事件</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NeedAction</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>需求道具</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RequireItem</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>种植课程</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>plant</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>需求</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>增项</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>zwwandou</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>zzwandou</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|奥莱伊李交了你种植植物的方法，||你需要到附近的田地里，种下|Y|豌豆种子||。并在收获后，把果实带交给他。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
+    <t>教训猩猩</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>onelesson</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞巴斯恰恩||委托你找到可恶的|G|科迪||，并通过卡牌战斗的方式击败他。|G|科迪|经常欺负周边的村民，非常可恶。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npckedi</t>
+  </si>
+  <si>
+    <t>questonelesson</t>
   </si>
 </sst>
 </file>
@@ -1304,6 +1322,31 @@
   </cellStyles>
   <dxfs count="12">
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
@@ -1366,31 +1409,6 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="2"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.39997558519241921"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1405,7 +1423,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AA14" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AA14" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A3:AA14"/>
   <sortState ref="A4:AA14">
     <sortCondition ref="A3:A14"/>
@@ -1421,8 +1439,8 @@
     <tableColumn id="13" name="Descript"/>
     <tableColumn id="20" name="NpcId"/>
     <tableColumn id="21" name="Type"/>
-    <tableColumn id="9" name="ResetOnLeave" dataDxfId="10"/>
-    <tableColumn id="23" name="TriggerSceneQuest" dataDxfId="9"/>
+    <tableColumn id="9" name="ResetOnLeave" dataDxfId="1"/>
+    <tableColumn id="23" name="TriggerSceneQuest" dataDxfId="0"/>
     <tableColumn id="7" name="CheckSceneQuest"/>
     <tableColumn id="27" name="ProgressAdd"/>
     <tableColumn id="8" name="QuestScript"/>
@@ -1767,7 +1785,7 @@
   <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1779,7 +1797,9 @@
     <col min="9" max="9" width="9.125" customWidth="1"/>
     <col min="10" max="11" width="7.375" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="19" max="27" width="7.5" customWidth="1"/>
+    <col min="14" max="14" width="5.625" customWidth="1"/>
+    <col min="19" max="26" width="7.5" customWidth="1"/>
+    <col min="27" max="27" width="9.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -1793,7 +1813,7 @@
         <v>32</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>7</v>
@@ -1817,25 +1837,25 @@
         <v>42</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M1" s="11" t="s">
         <v>54</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P1" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q1" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R1" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>9</v>
@@ -1876,7 +1896,7 @@
         <v>30</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>6</v>
@@ -1894,7 +1914,7 @@
         <v>34</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>43</v>
@@ -1906,19 +1926,19 @@
         <v>17</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>17</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="Q2" s="22" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>16</v>
@@ -1959,7 +1979,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
@@ -1980,28 +2000,28 @@
         <v>39</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="O3" s="13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="R3" s="24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>18</v>
@@ -2051,19 +2071,19 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I4">
         <v>42120001</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S4">
         <v>50</v>
@@ -2092,24 +2112,24 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="I5">
         <v>42120001</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N5">
         <v>10</v>
       </c>
       <c r="O5" t="s">
-        <v>57</v>
+        <v>110</v>
       </c>
       <c r="S5">
         <v>50</v>
@@ -2120,10 +2140,10 @@
         <v>12000003</v>
       </c>
       <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
         <v>66</v>
-      </c>
-      <c r="C6" t="s">
-        <v>67</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2135,20 +2155,20 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I6">
         <v>42120002</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K6" s="10"/>
       <c r="N6">
         <v>5</v>
       </c>
       <c r="P6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.15">
@@ -2156,10 +2176,10 @@
         <v>12000004</v>
       </c>
       <c r="B7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" t="s">
         <v>83</v>
-      </c>
-      <c r="C7" t="s">
-        <v>84</v>
       </c>
       <c r="D7">
         <v>12000003</v>
@@ -2174,13 +2194,13 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I7">
         <v>42120002</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
@@ -2188,7 +2208,7 @@
         <v>10</v>
       </c>
       <c r="P7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S7">
         <v>300</v>
@@ -2200,7 +2220,7 @@
         <v>300</v>
       </c>
       <c r="X7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.15">
@@ -2223,19 +2243,19 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I8">
         <v>42120003</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>44</v>
       </c>
       <c r="L8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="S8">
         <v>100</v>
@@ -2261,25 +2281,25 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I9">
         <v>42120005</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="Q9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S9">
         <v>100</v>
       </c>
       <c r="X9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.15">
@@ -2287,10 +2307,10 @@
         <v>12000007</v>
       </c>
       <c r="B10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C10" t="s">
         <v>89</v>
-      </c>
-      <c r="C10" t="s">
-        <v>90</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -2302,13 +2322,13 @@
         <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I10">
         <v>42120014</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
@@ -2321,10 +2341,10 @@
         <v>12000008</v>
       </c>
       <c r="B11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" t="s">
         <v>104</v>
-      </c>
-      <c r="C11" t="s">
-        <v>105</v>
       </c>
       <c r="D11">
         <v>12000006</v>
@@ -2339,26 +2359,32 @@
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I11">
         <v>42120005</v>
       </c>
       <c r="J11" s="25" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="R11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>12000009</v>
       </c>
-      <c r="B12">
+      <c r="B12" t="s">
         <v>111</v>
+      </c>
+      <c r="C12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12">
+        <v>12000005</v>
       </c>
       <c r="E12">
         <v>1</v>
@@ -2369,8 +2395,32 @@
       <c r="G12">
         <v>2</v>
       </c>
+      <c r="H12" t="s">
+        <v>113</v>
+      </c>
+      <c r="I12">
+        <v>42120003</v>
+      </c>
+      <c r="J12" s="18" t="s">
+        <v>106</v>
+      </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
+      <c r="M12" t="s">
+        <v>114</v>
+      </c>
+      <c r="N12">
+        <v>10</v>
+      </c>
+      <c r="O12" t="s">
+        <v>115</v>
+      </c>
+      <c r="S12">
+        <v>50</v>
+      </c>
+      <c r="AA12">
+        <v>43020103</v>
+      </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A13">
@@ -2383,7 +2433,7 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G13">
         <v>2</v>
@@ -2412,48 +2462,48 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="M9:AA14 A4:AA5 O6:AA6 O8:AA8 A7:G7 A8 A10:A11 A13:A14 K7:AA7 B8:L10 B12:L14 B11:C11 E11:L11">
-    <cfRule type="containsBlanks" dxfId="8" priority="10">
+  <conditionalFormatting sqref="M9:AA14 A4:AA5 O6:AA6 O8:AA8 A7:G7 A8 A10:A11 A13:A14 K7:AA7 B8:L10 B11:C11 E11:L11 B12:L14">
+    <cfRule type="containsBlanks" dxfId="11" priority="10">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8:N8">
-    <cfRule type="containsBlanks" dxfId="7" priority="8">
+    <cfRule type="containsBlanks" dxfId="10" priority="8">
       <formula>LEN(TRIM(M8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:G6 I6:L6 A9 A12">
-    <cfRule type="containsBlanks" dxfId="6" priority="7">
+    <cfRule type="containsBlanks" dxfId="9" priority="7">
       <formula>LEN(TRIM(A6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6:N6">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+    <cfRule type="containsBlanks" dxfId="8" priority="6">
       <formula>LEN(TRIM(M6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="7" priority="5">
       <formula>LEN(TRIM(H6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="6" priority="4">
       <formula>LEN(TRIM(J7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="5" priority="3">
       <formula>LEN(TRIM(I7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="4" priority="2">
       <formula>LEN(TRIM(H7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(D11))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
fix some task bugs
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -464,14 +464,14 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>G|塞巴斯恰恩||委托你找到可恶的|G|科迪||，并通过卡牌战斗的方式击败他。|G|科迪|经常欺负周边的村民，非常可恶。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>npckedi</t>
   </si>
   <si>
     <t>questonelesson</t>
+  </si>
+  <si>
+    <t>G|塞巴斯恰恩||委托你找到可恶的|G|科迪||，并通过卡牌战斗的方式击败他。|G|科迪||经常欺负周边的村民，非常可恶。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1785,7 +1785,7 @@
   <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2396,7 +2396,7 @@
         <v>2</v>
       </c>
       <c r="H12" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I12">
         <v>42120003</v>
@@ -2407,13 +2407,13 @@
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N12">
         <v>10</v>
       </c>
       <c r="O12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="S12">
         <v>50</v>

</xml_diff>

<commit_message>
add a new quest
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="124">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -360,10 +360,6 @@
     <t>G|玛莎||告诉你，他的孩子，前几天走失了。如果你碰到了这个孩子，一定要记得把他带回来</t>
   </si>
   <si>
-    <t>对话</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>走失的孩子</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -471,6 +467,39 @@
   </si>
   <si>
     <t>G|塞巴斯恰恩||委托你找到可恶的|G|科迪||，并通过卡牌战斗的方式击败他。|G|科迪||经常欺负周边的村民，非常可恶。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>遗迹村落</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lossviliage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>stonewords</t>
+  </si>
+  <si>
+    <t>G|科迪||告诉你，附近的|B|村落遗迹||中，隐藏着一些秘密，你可以去调查下，说不定会有意外的收获。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npckid1</t>
+  </si>
+  <si>
+    <t>bossmanwang</t>
+  </si>
+  <si>
+    <t>村落之主</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>viliageking</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|科迪||希望你可以找到并战胜|B|村落遗迹||中的|O|蛮王之灵||。</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -675,7 +704,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="49">
+  <fills count="48">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -930,12 +959,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1196,7 +1219,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1257,9 +1280,6 @@
     <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
@@ -1269,10 +1289,10 @@
     <xf numFmtId="0" fontId="21" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" textRotation="255"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1320,7 +1340,35 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1423,7 +1471,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AA14" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AA14" totalsRowShown="0" headerRowDxfId="6">
   <autoFilter ref="A3:AA14"/>
   <sortState ref="A4:AA14">
     <sortCondition ref="A3:A14"/>
@@ -1439,8 +1487,8 @@
     <tableColumn id="13" name="Descript"/>
     <tableColumn id="20" name="NpcId"/>
     <tableColumn id="21" name="Type"/>
-    <tableColumn id="9" name="ResetOnLeave" dataDxfId="1"/>
-    <tableColumn id="23" name="TriggerSceneQuest" dataDxfId="0"/>
+    <tableColumn id="9" name="ResetOnLeave" dataDxfId="5"/>
+    <tableColumn id="23" name="TriggerSceneQuest" dataDxfId="4"/>
     <tableColumn id="7" name="CheckSceneQuest"/>
     <tableColumn id="27" name="ProgressAdd"/>
     <tableColumn id="8" name="QuestScript"/>
@@ -1785,7 +1833,7 @@
   <dimension ref="A1:AA14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1851,11 +1899,11 @@
       <c r="P1" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="Q1" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="R1" s="23" t="s">
-        <v>101</v>
+      <c r="Q1" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="R1" s="22" t="s">
+        <v>100</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>9</v>
@@ -1934,11 +1982,11 @@
       <c r="P2" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="Q2" s="22" t="s">
-        <v>96</v>
+      <c r="Q2" s="21" t="s">
+        <v>95</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>16</v>
@@ -2000,7 +2048,7 @@
         <v>39</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L3" s="7" t="s">
         <v>74</v>
@@ -2018,10 +2066,10 @@
         <v>77</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>99</v>
-      </c>
-      <c r="R3" s="24" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="R3" s="23" t="s">
+        <v>101</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>18</v>
@@ -2085,6 +2133,12 @@
       <c r="L4" t="s">
         <v>72</v>
       </c>
+      <c r="N4">
+        <v>10</v>
+      </c>
+      <c r="P4" t="s">
+        <v>72</v>
+      </c>
       <c r="S4">
         <v>50</v>
       </c>
@@ -2118,7 +2172,7 @@
         <v>42120001</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
@@ -2129,7 +2183,7 @@
         <v>10</v>
       </c>
       <c r="O5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="S5">
         <v>50</v>
@@ -2155,7 +2209,7 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I6">
         <v>42120002</v>
@@ -2194,7 +2248,7 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I7">
         <v>42120002</v>
@@ -2243,7 +2297,7 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="I8">
         <v>42120003</v>
@@ -2255,6 +2309,12 @@
         <v>44</v>
       </c>
       <c r="L8" t="s">
+        <v>73</v>
+      </c>
+      <c r="N8">
+        <v>10</v>
+      </c>
+      <c r="P8" t="s">
         <v>73</v>
       </c>
       <c r="S8">
@@ -2281,25 +2341,25 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I9">
         <v>42120005</v>
       </c>
       <c r="J9" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="Q9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="S9">
         <v>100</v>
       </c>
       <c r="X9" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.15">
@@ -2307,10 +2367,10 @@
         <v>12000007</v>
       </c>
       <c r="B10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
         <v>88</v>
-      </c>
-      <c r="C10" t="s">
-        <v>89</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -2327,11 +2387,17 @@
       <c r="I10">
         <v>42120014</v>
       </c>
-      <c r="J10" s="20" t="s">
-        <v>87</v>
+      <c r="J10" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
+      <c r="N10">
+        <v>10</v>
+      </c>
+      <c r="P10" t="s">
+        <v>119</v>
+      </c>
       <c r="S10">
         <v>100</v>
       </c>
@@ -2341,10 +2407,10 @@
         <v>12000008</v>
       </c>
       <c r="B11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" t="s">
         <v>103</v>
-      </c>
-      <c r="C11" t="s">
-        <v>104</v>
       </c>
       <c r="D11">
         <v>12000006</v>
@@ -2359,18 +2425,18 @@
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="I11">
         <v>42120005</v>
       </c>
-      <c r="J11" s="25" t="s">
-        <v>105</v>
+      <c r="J11" s="24" t="s">
+        <v>104</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="R11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.15">
@@ -2378,10 +2444,10 @@
         <v>12000009</v>
       </c>
       <c r="B12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" t="s">
         <v>111</v>
-      </c>
-      <c r="C12" t="s">
-        <v>112</v>
       </c>
       <c r="D12">
         <v>12000005</v>
@@ -2390,30 +2456,30 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="G12">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="H12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I12">
         <v>42120003</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="N12">
         <v>10</v>
       </c>
       <c r="O12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S12">
         <v>50</v>
@@ -2426,85 +2492,156 @@
       <c r="A13">
         <v>12000010</v>
       </c>
-      <c r="B13">
-        <v>111</v>
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+      <c r="C13" t="s">
+        <v>116</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G13">
-        <v>2</v>
+        <v>5</v>
+      </c>
+      <c r="H13" t="s">
+        <v>118</v>
+      </c>
+      <c r="I13">
+        <v>42120006</v>
+      </c>
+      <c r="J13" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
+      <c r="N13">
+        <v>10</v>
+      </c>
+      <c r="P13" t="s">
+        <v>117</v>
+      </c>
+      <c r="S13">
+        <v>100</v>
+      </c>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>12000011</v>
       </c>
-      <c r="B14">
-        <v>111</v>
+      <c r="B14" t="s">
+        <v>121</v>
+      </c>
+      <c r="C14" t="s">
+        <v>122</v>
+      </c>
+      <c r="D14">
+        <v>12000010</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="G14">
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="H14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I14">
+        <v>42120006</v>
+      </c>
+      <c r="J14" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
+      <c r="N14">
+        <v>10</v>
+      </c>
+      <c r="P14" t="s">
+        <v>120</v>
+      </c>
+      <c r="S14">
+        <v>300</v>
+      </c>
+      <c r="U14">
+        <v>300</v>
+      </c>
+      <c r="V14">
+        <v>300</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="M9:AA14 A4:AA5 O6:AA6 O8:AA8 A7:G7 A8 A10:A11 A13:A14 K7:AA7 B8:L10 B11:C11 E11:L11 B12:L14">
-    <cfRule type="containsBlanks" dxfId="11" priority="10">
+  <conditionalFormatting sqref="M9:AA14 A4:AA5 O6:AA6 O8:AA8 A7:G7 A8 A10:A11 A13:A14 K7:AA7 B8:L9 B11:C11 E11:L11 B12:L12 B13:C13 E13:I13 B10:I10 K10:L10 K13:L14 B14:I14">
+    <cfRule type="containsBlanks" dxfId="15" priority="14">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8:N8">
-    <cfRule type="containsBlanks" dxfId="10" priority="8">
+    <cfRule type="containsBlanks" dxfId="14" priority="12">
       <formula>LEN(TRIM(M8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:G6 I6:L6 A9 A12">
-    <cfRule type="containsBlanks" dxfId="9" priority="7">
+    <cfRule type="containsBlanks" dxfId="13" priority="11">
       <formula>LEN(TRIM(A6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6:N6">
-    <cfRule type="containsBlanks" dxfId="8" priority="6">
+    <cfRule type="containsBlanks" dxfId="12" priority="10">
       <formula>LEN(TRIM(M6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="containsBlanks" dxfId="7" priority="5">
+    <cfRule type="containsBlanks" dxfId="11" priority="9">
       <formula>LEN(TRIM(H6))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J7">
-    <cfRule type="containsBlanks" dxfId="6" priority="4">
+    <cfRule type="containsBlanks" dxfId="10" priority="8">
       <formula>LEN(TRIM(J7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="containsBlanks" dxfId="5" priority="3">
+    <cfRule type="containsBlanks" dxfId="9" priority="7">
       <formula>LEN(TRIM(I7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7">
-    <cfRule type="containsBlanks" dxfId="4" priority="2">
+    <cfRule type="containsBlanks" dxfId="8" priority="6">
       <formula>LEN(TRIM(H7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D11">
-    <cfRule type="containsBlanks" dxfId="3" priority="1">
+    <cfRule type="containsBlanks" dxfId="7" priority="5">
       <formula>LEN(TRIM(D11))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D13">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(D13))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J13">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(J13))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J10">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(J10))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J14">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(J14))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
use string to index people table
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="124">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -106,10 +106,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>RivalId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>生命奖励系数</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -118,23 +114,200 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>RewardFood</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardHealth</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardItem</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RewardDrop</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ename</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>英文名</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务npc</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>RewardFood</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardHealth</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardItem</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RewardDrop</t>
+    <t>NpcId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>名字</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>序列</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>开始</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>恰恰</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>离开地图重置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>清理农场</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectjob</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiaqia</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>aolai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>影响sq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>采集罂粟</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pickpoppy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield</t>
+  </si>
+  <si>
+    <t>交互的脚本</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestScript</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>前置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Former</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|乔斯基||让你去找|G|瓦里斯||，并向他学习战斗的技巧，提升自己。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|乔斯基||需要一些罂粟花苗，让你寻找收集一些。应该可以从|O|罂粟花田||中找到。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>狼群的威胁</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfflow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>进度变化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProgressAdd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发sq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcwalisi</t>
+  </si>
+  <si>
+    <t>npcqiaqia</t>
+  </si>
+  <si>
+    <t>TriggerSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成sq</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -142,55 +315,88 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Ename</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>英文名</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>任务npc</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NpcId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>名字</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>序列</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>任务类型</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>开始</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>恰恰</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>离开地图重置</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
+    <t>SuccessSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>成功</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>穷奇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiongqi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossqiongqi</t>
+  </si>
+  <si>
+    <t>rwqiongqi</t>
+  </si>
+  <si>
+    <t>G|玛莎||告诉你，他的孩子，前几天走失了。如果你碰到了这个孩子，一定要记得把他带回来</t>
+  </si>
+  <si>
+    <t>走失的孩子</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lossboy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞尼斯||希望你帮助他，进入附近的|O|狼穴||并消灭狼群，如果失败了，你可以尝试反复进出本地图重试。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞尼斯||告诉你，再附近的森林深处，有一只神兽|O|穷奇||，如果你可以找到并击败他，会得到丰厚的回报。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞巴斯恰恩||的宠物|G|恰恰||不见了，他希望你可以帮助他找回宠物。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|奥莱伊李||觉得目前的田野很不安全，希望你可以帮助他清理当前场景的所有特殊事件。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResetOnLeave</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件触发</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>allopen</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedAction</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
@@ -198,220 +404,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>清理农场</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>selectjob</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>qiaqia</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>aolai</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>显示x</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>显示y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>影响sq</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>采集罂粟</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>pickpoppy</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>poppyfield</t>
-  </si>
-  <si>
-    <t>交互的脚本</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QuestScript</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>前置</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Former</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|乔斯基||让你去找|G|瓦里斯||，并向他学习战斗的技巧，提升自己。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|乔斯基||需要一些罂粟花苗，让你寻找收集一些。应该可以从|O|罂粟花田||中找到。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>狼群的威胁</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfflow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>进度变化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ProgressAdd</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>CheckSceneQuest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>触发sq</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npcwalisi</t>
-  </si>
-  <si>
-    <t>npcqiaqia</t>
-  </si>
-  <si>
-    <t>TriggerSceneQuest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成sq</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SuccessSceneQuest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfnest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>触发</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>成功</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>穷奇</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>qiongqi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bossqiongqi</t>
-  </si>
-  <si>
-    <t>rwqiongqi</t>
-  </si>
-  <si>
-    <t>G|玛莎||告诉你，他的孩子，前几天走失了。如果你碰到了这个孩子，一定要记得把他带回来</t>
-  </si>
-  <si>
-    <t>走失的孩子</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>lossboy</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|塞尼斯||希望你帮助他，进入附近的|O|狼穴||并消灭狼群，如果失败了，你可以尝试反复进出本地图重试。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|塞尼斯||告诉你，再附近的森林深处，有一只神兽|O|穷奇||，如果你可以找到并击败他，会得到丰厚的回报。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|塞巴斯恰恩||的宠物|G|恰恰||不见了，他希望你可以帮助他找回宠物。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|奥莱伊李||觉得目前的田野很不安全，希望你可以帮助他清理当前场景的所有特殊事件。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ResetOnLeave</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>事件触发</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>allopen</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>事件</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NeedAction</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>需求道具</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -500,6 +492,13 @@
   </si>
   <si>
     <t>G|科迪||希望你可以找到并战胜|B|村落遗迹||中的|O|蛮王之灵||。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>weia</t>
+  </si>
+  <si>
+    <t>UnlockRival</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -975,7 +974,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1090,6 +1089,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1219,7 +1227,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1293,6 +1301,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1341,34 +1352,6 @@
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
@@ -1457,6 +1440,34 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1471,7 +1482,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AA14" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AA14" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A3:AA14"/>
   <sortState ref="A4:AA14">
     <sortCondition ref="A3:A14"/>
@@ -1487,8 +1498,8 @@
     <tableColumn id="13" name="Descript"/>
     <tableColumn id="20" name="NpcId"/>
     <tableColumn id="21" name="Type"/>
-    <tableColumn id="9" name="ResetOnLeave" dataDxfId="5"/>
-    <tableColumn id="23" name="TriggerSceneQuest" dataDxfId="4"/>
+    <tableColumn id="9" name="ResetOnLeave" dataDxfId="1"/>
+    <tableColumn id="23" name="TriggerSceneQuest" dataDxfId="0"/>
     <tableColumn id="7" name="CheckSceneQuest"/>
     <tableColumn id="27" name="ProgressAdd"/>
     <tableColumn id="8" name="QuestScript"/>
@@ -1503,7 +1514,7 @@
     <tableColumn id="15" name="RewardItem"/>
     <tableColumn id="16" name="RewardDrop"/>
     <tableColumn id="17" name="RewardBlessLevel"/>
-    <tableColumn id="18" name="RivalId"/>
+    <tableColumn id="18" name="UnlockRival"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1832,8 +1843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="AA3" sqref="AA3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1852,58 +1863,58 @@
   <sheetData>
     <row r="1" spans="1:27" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="P1" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="Q1" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="R1" s="22" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="S1" s="4" t="s">
         <v>9</v>
@@ -1912,7 +1923,7 @@
         <v>10</v>
       </c>
       <c r="U1" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="V1" s="4" t="s">
         <v>11</v>
@@ -1924,7 +1935,7 @@
         <v>13</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="4" t="s">
         <v>14</v>
@@ -1941,31 +1952,31 @@
         <v>1</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>1</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L2" s="5" t="s">
         <v>1</v>
@@ -1974,19 +1985,19 @@
         <v>17</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="O2" s="12" t="s">
         <v>17</v>
       </c>
       <c r="P2" s="15" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="Q2" s="21" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="S2" s="6" t="s">
         <v>16</v>
@@ -2013,7 +2024,7 @@
         <v>0</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.15">
@@ -2024,61 +2035,61 @@
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J3" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L3" s="7" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M3" s="13" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O3" s="13" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="P3" s="16" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q3" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="R3" s="23" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="S3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>19</v>
@@ -2087,16 +2098,16 @@
         <v>20</v>
       </c>
       <c r="X3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="Z3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>22</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.15">
@@ -2104,10 +2115,10 @@
         <v>12000001</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2119,25 +2130,25 @@
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I4">
         <v>42120001</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N4">
         <v>10</v>
       </c>
       <c r="P4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="S4">
         <v>50</v>
@@ -2148,10 +2159,10 @@
         <v>12000002</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D5">
         <v>12000001</v>
@@ -2166,24 +2177,24 @@
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="I5">
         <v>42120001</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N5">
         <v>10</v>
       </c>
       <c r="O5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="S5">
         <v>50</v>
@@ -2194,10 +2205,10 @@
         <v>12000003</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E6">
         <v>1</v>
@@ -2209,20 +2220,20 @@
         <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="I6">
         <v>42120002</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K6" s="10"/>
       <c r="N6">
         <v>5</v>
       </c>
       <c r="P6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.15">
@@ -2230,10 +2241,10 @@
         <v>12000004</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D7">
         <v>12000003</v>
@@ -2248,13 +2259,13 @@
         <v>6</v>
       </c>
       <c r="H7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="I7">
         <v>42120002</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="10"/>
@@ -2262,7 +2273,7 @@
         <v>10</v>
       </c>
       <c r="P7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="S7">
         <v>300</v>
@@ -2274,7 +2285,7 @@
         <v>300</v>
       </c>
       <c r="X7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.15">
@@ -2282,10 +2293,10 @@
         <v>12000005</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2297,25 +2308,25 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I8">
         <v>42120003</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="N8">
         <v>10</v>
       </c>
       <c r="P8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="S8">
         <v>100</v>
@@ -2326,10 +2337,10 @@
         <v>12000006</v>
       </c>
       <c r="B9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2341,25 +2352,25 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I9">
         <v>42120005</v>
       </c>
       <c r="J9" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="K9" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="K9" s="10" t="s">
-        <v>99</v>
-      </c>
       <c r="Q9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S9">
         <v>100</v>
       </c>
       <c r="X9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.15">
@@ -2367,10 +2378,10 @@
         <v>12000007</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -2382,13 +2393,13 @@
         <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I10">
         <v>42120014</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="10"/>
@@ -2396,7 +2407,7 @@
         <v>10</v>
       </c>
       <c r="P10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="S10">
         <v>100</v>
@@ -2407,10 +2418,10 @@
         <v>12000008</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D11">
         <v>12000006</v>
@@ -2425,18 +2436,18 @@
         <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="I11">
         <v>42120005</v>
       </c>
       <c r="J11" s="24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="10"/>
       <c r="R11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.15">
@@ -2444,10 +2455,10 @@
         <v>12000009</v>
       </c>
       <c r="B12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C12" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D12">
         <v>12000005</v>
@@ -2462,30 +2473,30 @@
         <v>7</v>
       </c>
       <c r="H12" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="I12">
         <v>42120003</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="10"/>
       <c r="M12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="N12">
         <v>10</v>
       </c>
       <c r="O12" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="S12">
         <v>50</v>
       </c>
-      <c r="AA12">
-        <v>43020103</v>
+      <c r="AA12" s="25" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.15">
@@ -2493,10 +2504,10 @@
         <v>12000010</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -2508,13 +2519,13 @@
         <v>5</v>
       </c>
       <c r="H13" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I13">
         <v>42120006</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="10"/>
@@ -2522,7 +2533,7 @@
         <v>10</v>
       </c>
       <c r="P13" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="S13">
         <v>100</v>
@@ -2533,10 +2544,10 @@
         <v>12000011</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D14">
         <v>12000010</v>
@@ -2551,13 +2562,13 @@
         <v>8</v>
       </c>
       <c r="H14" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I14">
         <v>42120006</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="10"/>
@@ -2565,7 +2576,7 @@
         <v>10</v>
       </c>
       <c r="P14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="S14">
         <v>300</v>
@@ -2625,22 +2636,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D13">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="6" priority="4">
       <formula>LEN(TRIM(D13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J13">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+    <cfRule type="containsBlanks" dxfId="5" priority="3">
       <formula>LEN(TRIM(J13))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J10">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="4" priority="2">
       <formula>LEN(TRIM(J10))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="3" priority="1">
       <formula>LEN(TRIM(J14))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
optimise the quest show effect
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -18,8 +18,81 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Real</author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>Real:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>0</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t xml:space="preserve">.主线
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <family val="3"/>
+            <charset val="134"/>
+          </rPr>
+          <t>1</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="宋体"/>
+            <charset val="134"/>
+          </rPr>
+          <t>.支线</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="135">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -142,18 +215,10 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>任务npc</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>NpcId</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>名字</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -166,339 +231,390 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
+    <t>开始</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>恰恰</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>离开地图重置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bool</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>清理农场</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectjob</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiaqia</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>aolai</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示x</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>显示y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>X</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Y</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>影响sq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>采集罂粟</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>pickpoppy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>poppyfield</t>
+  </si>
+  <si>
+    <t>交互的脚本</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>QuestScript</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>前置</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Former</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|乔斯基||让你去找|G|瓦里斯||，并向他学习战斗的技巧，提升自己。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|乔斯基||需要一些罂粟花苗，让你寻找收集一些。应该可以从|O|罂粟花田||中找到。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>狼群的威胁</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfflow</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>进度变化</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ProgressAdd</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>CheckSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发sq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npcwalisi</t>
+  </si>
+  <si>
+    <t>npcqiaqia</t>
+  </si>
+  <si>
+    <t>TriggerSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>完成sq</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>SuccessSceneQuest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>wolfnest</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>触发</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>成功</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>穷奇</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>qiongqi</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>bossqiongqi</t>
+  </si>
+  <si>
+    <t>rwqiongqi</t>
+  </si>
+  <si>
+    <t>G|玛莎||告诉你，他的孩子，前几天走失了。如果你碰到了这个孩子，一定要记得把他带回来</t>
+  </si>
+  <si>
+    <t>走失的孩子</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lossboy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞尼斯||希望你帮助他，进入附近的|O|狼穴||并消灭狼群，如果失败了，你可以尝试反复进出本地图重试。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞尼斯||告诉你，再附近的森林深处，有一只神兽|O|穷奇||，如果你可以找到并击败他，会得到丰厚的回报。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|塞巴斯恰恩||的宠物|G|恰恰||不见了，他希望你可以帮助他找回宠物。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|奥莱伊李||觉得目前的田野很不安全，希望你可以帮助他清理当前场景的所有特殊事件。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResetOnLeave</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件触发</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>allopen</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>事件</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>NeedAction</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求道具</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RequireItem</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>种植课程</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>plant</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>增项</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zwwandou</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>zzwandou</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|奥莱伊李||教了你种植植物的方法，||你需要到附近的田地里，种下|Y|豌豆种子||。并在收获后，把果实带交给他。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>questpickpoppy</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>教训猩猩</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>onelesson</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npckedi</t>
+  </si>
+  <si>
+    <t>questonelesson</t>
+  </si>
+  <si>
+    <t>G|塞巴斯恰恩||委托你找到可恶的|G|科迪||，并通过卡牌战斗的方式击败他。|G|科迪||经常欺负周边的村民，非常可恶。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>遗迹村落</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>lossviliage</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>stonewords</t>
+  </si>
+  <si>
+    <t>G|科迪||告诉你，附近的|B|村落遗迹||中，隐藏着一些秘密，你可以去调查下，说不定会有意外的收获。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>npckid1</t>
+  </si>
+  <si>
+    <t>bossmanwang</t>
+  </si>
+  <si>
+    <t>村落之主</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>viliageking</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|科迪||希望你可以找到并战胜|B|村落遗迹||中的|O|蛮王之灵||。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>weia</t>
+  </si>
+  <si>
+    <t>UnlockRival</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务类型</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
     <t>Type</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>开始</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>恰恰</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>离开地图重置</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bool</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>清理农场</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>selectjob</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>qiaqia</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>aolai</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>显示x</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>显示y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>X</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Y</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>影响sq</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>采集罂粟</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>pickpoppy</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>poppyfield</t>
-  </si>
-  <si>
-    <t>交互的脚本</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>QuestScript</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>前置</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>Former</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|乔斯基||让你去找|G|瓦里斯||，并向他学习战斗的技巧，提升自己。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|乔斯基||需要一些罂粟花苗，让你寻找收集一些。应该可以从|O|罂粟花田||中找到。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>狼群的威胁</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfflow</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>进度变化</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>int</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ProgressAdd</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>CheckSceneQuest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>触发sq</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npcwalisi</t>
-  </si>
-  <si>
-    <t>npcqiaqia</t>
-  </si>
-  <si>
-    <t>TriggerSceneQuest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成sq</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>SuccessSceneQuest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>wolfnest</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>触发</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>成功</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>穷奇</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>qiongqi</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>bossqiongqi</t>
-  </si>
-  <si>
-    <t>rwqiongqi</t>
-  </si>
-  <si>
-    <t>G|玛莎||告诉你，他的孩子，前几天走失了。如果你碰到了这个孩子，一定要记得把他带回来</t>
-  </si>
-  <si>
-    <t>走失的孩子</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>lossboy</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|塞尼斯||希望你帮助他，进入附近的|O|狼穴||并消灭狼群，如果失败了，你可以尝试反复进出本地图重试。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|塞尼斯||告诉你，再附近的森林深处，有一只神兽|O|穷奇||，如果你可以找到并击败他，会得到丰厚的回报。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|塞巴斯恰恩||的宠物|G|恰恰||不见了，他希望你可以帮助他找回宠物。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|奥莱伊李||觉得目前的田野很不安全，希望你可以帮助他清理当前场景的所有特殊事件。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>ResetOnLeave</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>事件触发</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>allopen</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>事件</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>NeedAction</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>true</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>需求道具</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>RequireItem</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>种植课程</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>plant</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>需求</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>增项</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>zwwandou</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>zzwandou</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|奥莱伊李||教了你种植植物的方法，||你需要到附近的田地里，种下|Y|豌豆种子||。并在收获后，把果实带交给他。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>questpickpoppy</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>教训猩猩</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>onelesson</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npckedi</t>
-  </si>
-  <si>
-    <t>questonelesson</t>
-  </si>
-  <si>
-    <t>G|塞巴斯恰恩||委托你找到可恶的|G|科迪||，并通过卡牌战斗的方式击败他。|G|科迪||经常欺负周边的村民，非常可恶。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>遗迹村落</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>lossviliage</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>stonewords</t>
-  </si>
-  <si>
-    <t>G|科迪||告诉你，附近的|B|村落遗迹||中，隐藏着一些秘密，你可以去调查下，说不定会有意外的收获。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>npckid1</t>
-  </si>
-  <si>
-    <t>bossmanwang</t>
-  </si>
-  <si>
-    <t>村落之主</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>viliageking</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|科迪||希望你可以找到并战胜|B|村落遗迹||中的|O|蛮王之灵||。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>weia</t>
-  </si>
-  <si>
-    <t>UnlockRival</t>
+    <t>目标</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>target</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|乔斯基||希望你可以去到|B|布萨特高塔||，并在那里历练自己。</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>StartNpcId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>接任务npc</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>EndNpcId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务提交npc</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>需求场景</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>RequireSceneId</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>kapaibugeibao(an)</t>
+  </si>
+  <si>
+    <t>TypeR</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -506,7 +622,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -702,6 +818,26 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="48">
     <fill>
@@ -1227,7 +1363,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1236,12 +1372,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
@@ -1261,50 +1391,62 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" textRotation="255" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1351,29 +1493,11 @@
     <cellStyle name="着色 6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="19">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="2"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.39997558519241921"/>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1468,6 +1592,45 @@
         </patternFill>
       </fill>
     </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="2"/>
+        <name val="宋体"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1482,30 +1645,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AA14" totalsRowShown="0" headerRowDxfId="2">
-  <autoFilter ref="A3:AA14"/>
-  <sortState ref="A4:AA14">
-    <sortCondition ref="A3:A14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="表2" displayName="表2" ref="A3:AD15" totalsRowShown="0" headerRowDxfId="18">
+  <autoFilter ref="A3:AD15"/>
+  <sortState ref="A4:AD15">
+    <sortCondition ref="A3:A15"/>
   </sortState>
-  <tableColumns count="27">
+  <tableColumns count="30">
     <tableColumn id="1" name="Id"/>
     <tableColumn id="2" name="Name"/>
     <tableColumn id="19" name="Ename"/>
     <tableColumn id="25" name="Former"/>
+    <tableColumn id="26" name="TypeR"/>
     <tableColumn id="4" name="RegionId"/>
     <tableColumn id="22" name="X"/>
     <tableColumn id="24" name="Y"/>
     <tableColumn id="13" name="Descript"/>
-    <tableColumn id="20" name="NpcId"/>
+    <tableColumn id="20" name="StartNpcId"/>
+    <tableColumn id="29" name="EndNpcId"/>
     <tableColumn id="21" name="Type"/>
-    <tableColumn id="9" name="ResetOnLeave" dataDxfId="1"/>
-    <tableColumn id="23" name="TriggerSceneQuest" dataDxfId="0"/>
+    <tableColumn id="9" name="ResetOnLeave" dataDxfId="17"/>
+    <tableColumn id="23" name="TriggerSceneQuest" dataDxfId="16"/>
     <tableColumn id="7" name="CheckSceneQuest"/>
     <tableColumn id="27" name="ProgressAdd"/>
     <tableColumn id="8" name="QuestScript"/>
     <tableColumn id="28" name="SuccessSceneQuest"/>
     <tableColumn id="5" name="NeedAction"/>
     <tableColumn id="6" name="RequireItem"/>
+    <tableColumn id="30" name="RequireSceneId"/>
     <tableColumn id="10" name="RewardGold"/>
     <tableColumn id="3" name="RewardFood"/>
     <tableColumn id="11" name="RewardHealth"/>
@@ -1840,194 +2006,213 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.75" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="4.375" customWidth="1"/>
-    <col min="8" max="8" width="69.5" customWidth="1"/>
-    <col min="9" max="9" width="9.125" customWidth="1"/>
-    <col min="10" max="11" width="7.375" customWidth="1"/>
-    <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="14" max="14" width="5.625" customWidth="1"/>
-    <col min="19" max="26" width="7.5" customWidth="1"/>
-    <col min="27" max="27" width="9.25" customWidth="1"/>
+    <col min="5" max="8" width="4.375" customWidth="1"/>
+    <col min="9" max="9" width="69.5" customWidth="1"/>
+    <col min="10" max="11" width="9.125" customWidth="1"/>
+    <col min="12" max="13" width="7.375" customWidth="1"/>
+    <col min="14" max="14" width="9" customWidth="1"/>
+    <col min="16" max="16" width="5.625" customWidth="1"/>
+    <col min="21" max="21" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="29" width="7.5" customWidth="1"/>
+    <col min="30" max="30" width="9.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="8" t="s">
+    <row r="1" spans="1:30" ht="60.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="K1" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="L1" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" s="8" t="s">
+      <c r="M1" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="O1" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="S1" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="T1" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="U1" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="V1" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="W1" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="X1" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y1" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="Z1" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA1" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="AB1" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="AC1" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD1" s="27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="O1" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="P1" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q1" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="R1" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="S1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="T1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="U1" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="V1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="W1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="X1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="AA1" s="4" t="s">
-        <v>15</v>
+      <c r="K2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="S2" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="U2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="4" t="s">
+        <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A2" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="P2" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="Q2" s="21" t="s">
-        <v>93</v>
-      </c>
-      <c r="R2" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="T2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="X2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -2038,90 +2223,96 @@
         <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="L3" s="7" t="s">
+      <c r="J3" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="L3" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="M3" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="N3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="P3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="R3" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="M3" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="N3" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="P3" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q3" s="16" t="s">
+      <c r="S3" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="T3" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="R3" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="S3" s="2" t="s">
+      <c r="U3" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="V3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="2" t="s">
+      <c r="W3" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="U3" s="2" t="s">
+      <c r="X3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="V3" s="2" t="s">
+      <c r="Y3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W3" s="2" t="s">
+      <c r="Z3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="X3" s="2" t="s">
+      <c r="AA3" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="Y3" s="2" t="s">
+      <c r="AB3" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Z3" s="2" t="s">
+      <c r="AC3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="AA3" s="2" t="s">
-        <v>123</v>
+      <c r="AD3" s="2" t="s">
+        <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>12000001</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="F4">
         <v>1</v>
@@ -2129,548 +2320,638 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4">
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4">
         <v>42120001</v>
       </c>
-      <c r="J4" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="K4" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="L4" t="s">
-        <v>70</v>
-      </c>
-      <c r="N4">
+      <c r="L4" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N4" t="s">
+        <v>67</v>
+      </c>
+      <c r="P4">
         <v>10</v>
       </c>
-      <c r="P4" t="s">
-        <v>70</v>
-      </c>
-      <c r="S4">
+      <c r="R4" t="s">
+        <v>67</v>
+      </c>
+      <c r="V4">
         <v>50</v>
       </c>
-      <c r="W4">
+      <c r="Z4">
         <v>600</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>12000002</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>54</v>
+        <v>125</v>
       </c>
       <c r="D5">
         <v>12000001</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>3</v>
       </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
-        <v>62</v>
-      </c>
-      <c r="I5">
+      <c r="H5">
+        <v>7</v>
+      </c>
+      <c r="I5" t="s">
+        <v>126</v>
+      </c>
+      <c r="J5">
         <v>42120001</v>
       </c>
-      <c r="J5" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" t="s">
-        <v>55</v>
-      </c>
-      <c r="N5">
-        <v>10</v>
-      </c>
-      <c r="O5" t="s">
-        <v>107</v>
-      </c>
-      <c r="S5">
-        <v>50</v>
-      </c>
-      <c r="W5">
-        <v>600</v>
+      <c r="K5">
+        <v>42130031</v>
+      </c>
+      <c r="L5" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="U5">
+        <v>13010005</v>
+      </c>
+      <c r="V5">
+        <v>100</v>
+      </c>
+      <c r="X5">
+        <v>200</v>
+      </c>
+      <c r="Y5">
+        <v>200</v>
+      </c>
+      <c r="Z5">
+        <v>500</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>133</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>12000003</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6">
+        <v>61</v>
+      </c>
+      <c r="F6">
         <v>1</v>
-      </c>
-      <c r="F6">
-        <v>4</v>
       </c>
       <c r="G6">
         <v>4</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J6">
+        <v>42120002</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="M6" s="8"/>
+      <c r="P6">
+        <v>5</v>
+      </c>
+      <c r="R6" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>12000005</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7">
+        <v>42120003</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="N7" t="s">
+        <v>68</v>
+      </c>
+      <c r="P7">
+        <v>10</v>
+      </c>
+      <c r="R7" t="s">
+        <v>68</v>
+      </c>
+      <c r="V7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>12000006</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8" t="s">
         <v>87</v>
       </c>
-      <c r="I6">
-        <v>42120002</v>
-      </c>
-      <c r="J6" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K6" s="10"/>
-      <c r="N6">
+      <c r="J8">
+        <v>42120005</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="M8" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="S8" t="s">
+        <v>91</v>
+      </c>
+      <c r="V8">
+        <v>100</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>12000007</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
+        <v>3</v>
+      </c>
+      <c r="I9" t="s">
+        <v>81</v>
+      </c>
+      <c r="J9">
+        <v>42120014</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="P9">
+        <v>10</v>
+      </c>
+      <c r="R9" t="s">
+        <v>114</v>
+      </c>
+      <c r="V9">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>12000010</v>
+      </c>
+      <c r="B10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" t="s">
+        <v>111</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>10</v>
+      </c>
+      <c r="H10">
         <v>5</v>
       </c>
-      <c r="P6" t="s">
+      <c r="I10" t="s">
+        <v>113</v>
+      </c>
+      <c r="J10">
+        <v>42120006</v>
+      </c>
+      <c r="L10" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="W6">
-        <v>500</v>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="P10">
+        <v>10</v>
+      </c>
+      <c r="R10" t="s">
+        <v>112</v>
+      </c>
+      <c r="V10">
+        <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A7">
-        <v>12000004</v>
-      </c>
-      <c r="B7" t="s">
-        <v>80</v>
-      </c>
-      <c r="C7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7">
-        <v>12000003</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>7</v>
-      </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-      <c r="H7" t="s">
-        <v>88</v>
-      </c>
-      <c r="I7">
-        <v>42120002</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="N7">
-        <v>10</v>
-      </c>
-      <c r="P7" t="s">
-        <v>82</v>
-      </c>
-      <c r="S7">
-        <v>300</v>
-      </c>
-      <c r="U7">
-        <v>300</v>
-      </c>
-      <c r="V7">
-        <v>300</v>
-      </c>
-      <c r="W7">
-        <v>500</v>
-      </c>
-      <c r="X7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>12000005</v>
-      </c>
-      <c r="B8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C8" t="s">
-        <v>45</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>5</v>
-      </c>
-      <c r="G8">
-        <v>5</v>
-      </c>
-      <c r="H8" t="s">
-        <v>89</v>
-      </c>
-      <c r="I8">
-        <v>42120003</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>78</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="L8" t="s">
-        <v>71</v>
-      </c>
-      <c r="N8">
-        <v>10</v>
-      </c>
-      <c r="P8" t="s">
-        <v>71</v>
-      </c>
-      <c r="S8">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A9">
-        <v>12000006</v>
-      </c>
-      <c r="B9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>6</v>
-      </c>
-      <c r="G9">
-        <v>3</v>
-      </c>
-      <c r="H9" t="s">
-        <v>90</v>
-      </c>
-      <c r="I9">
-        <v>42120005</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>94</v>
-      </c>
-      <c r="S9">
-        <v>100</v>
-      </c>
-      <c r="X9" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <v>12000007</v>
-      </c>
-      <c r="B10" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" t="s">
-        <v>86</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <v>3</v>
-      </c>
-      <c r="H10" t="s">
-        <v>84</v>
-      </c>
-      <c r="I10">
-        <v>42120014</v>
-      </c>
-      <c r="J10" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="N10">
-        <v>10</v>
-      </c>
-      <c r="P10" t="s">
-        <v>117</v>
-      </c>
-      <c r="S10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A11">
-        <v>12000008</v>
+        <v>12000101</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="D11">
-        <v>12000006</v>
+        <v>12000001</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
       <c r="F11">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G11">
-        <v>2</v>
-      </c>
-      <c r="H11" t="s">
-        <v>106</v>
-      </c>
-      <c r="I11">
-        <v>42120005</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="R11" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11">
+        <v>42120001</v>
+      </c>
+      <c r="L11" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" t="s">
+        <v>52</v>
+      </c>
+      <c r="P11">
+        <v>10</v>
+      </c>
+      <c r="Q11" t="s">
         <v>104</v>
       </c>
+      <c r="V11">
+        <v>50</v>
+      </c>
+      <c r="Z11">
+        <v>600</v>
+      </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A12">
-        <v>12000009</v>
+        <v>12000102</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="D12">
-        <v>12000005</v>
+        <v>12000003</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
       <c r="F12">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G12">
         <v>7</v>
       </c>
-      <c r="H12" t="s">
-        <v>112</v>
-      </c>
-      <c r="I12">
-        <v>42120003</v>
-      </c>
-      <c r="J12" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" t="s">
-        <v>110</v>
-      </c>
-      <c r="N12">
+      <c r="H12">
+        <v>6</v>
+      </c>
+      <c r="I12" t="s">
+        <v>85</v>
+      </c>
+      <c r="J12">
+        <v>42120002</v>
+      </c>
+      <c r="L12" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="P12">
         <v>10</v>
       </c>
-      <c r="O12" t="s">
-        <v>111</v>
-      </c>
-      <c r="S12">
-        <v>50</v>
-      </c>
-      <c r="AA12" s="25" t="s">
-        <v>122</v>
+      <c r="R12" t="s">
+        <v>79</v>
+      </c>
+      <c r="V12">
+        <v>300</v>
+      </c>
+      <c r="X12">
+        <v>300</v>
+      </c>
+      <c r="Y12">
+        <v>300</v>
+      </c>
+      <c r="Z12">
+        <v>500</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>80</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A13">
-        <v>12000010</v>
+        <v>12000103</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>97</v>
       </c>
       <c r="C13" t="s">
-        <v>114</v>
+        <v>98</v>
+      </c>
+      <c r="D13">
+        <v>12000006</v>
       </c>
       <c r="E13">
         <v>1</v>
       </c>
       <c r="F13">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>5</v>
-      </c>
-      <c r="H13" t="s">
-        <v>116</v>
-      </c>
-      <c r="I13">
-        <v>42120006</v>
-      </c>
-      <c r="J13" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="N13">
-        <v>10</v>
-      </c>
-      <c r="P13" t="s">
-        <v>115</v>
-      </c>
-      <c r="S13">
-        <v>100</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13" t="s">
+        <v>103</v>
+      </c>
+      <c r="J13">
+        <v>42120005</v>
+      </c>
+      <c r="L13" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="T13" t="s">
+        <v>101</v>
+      </c>
+      <c r="AD13" s="20"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.15">
       <c r="A14">
-        <v>12000011</v>
+        <v>12000104</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="C14" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="D14">
-        <v>12000010</v>
+        <v>12000005</v>
       </c>
       <c r="E14">
         <v>1</v>
       </c>
       <c r="F14">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="G14">
         <v>8</v>
       </c>
-      <c r="H14" t="s">
-        <v>121</v>
-      </c>
-      <c r="I14">
+      <c r="H14">
+        <v>7</v>
+      </c>
+      <c r="I14" t="s">
+        <v>109</v>
+      </c>
+      <c r="J14">
+        <v>42120003</v>
+      </c>
+      <c r="L14" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" t="s">
+        <v>107</v>
+      </c>
+      <c r="P14">
+        <v>10</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>108</v>
+      </c>
+      <c r="V14">
+        <v>50</v>
+      </c>
+      <c r="AD14" s="19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.15">
+      <c r="A15">
+        <v>12000105</v>
+      </c>
+      <c r="B15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15">
+        <v>12000010</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>13</v>
+      </c>
+      <c r="H15">
+        <v>8</v>
+      </c>
+      <c r="I15" t="s">
+        <v>118</v>
+      </c>
+      <c r="J15">
         <v>42120006</v>
       </c>
-      <c r="J14" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="N14">
+      <c r="L15" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="P15">
         <v>10</v>
       </c>
-      <c r="P14" t="s">
-        <v>118</v>
-      </c>
-      <c r="S14">
+      <c r="R15" t="s">
+        <v>115</v>
+      </c>
+      <c r="V15">
         <v>300</v>
       </c>
-      <c r="U14">
+      <c r="X15">
         <v>300</v>
       </c>
-      <c r="V14">
+      <c r="Y15">
         <v>300</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <conditionalFormatting sqref="M9:AA14 A4:AA5 O6:AA6 O8:AA8 A7:G7 A8 A10:A11 A13:A14 K7:AA7 B8:L9 B11:C11 E11:L11 B12:L12 B13:C13 E13:I13 B10:I10 K10:L10 K13:L14 B14:I14">
-    <cfRule type="containsBlanks" dxfId="15" priority="14">
+  <conditionalFormatting sqref="O10:AD15 Q7:AD7 Q9:AD9 A8:H8 A9 M8:AD8 B12:C12 F12:J12 B13:J13 B14:C14 F14:J14 B9:J11 M11:N11 M14:N15 B15:J15 E11:E15 A11:A15 A4:J6 L12:N13 L9:N10 L4:AD6">
+    <cfRule type="containsBlanks" dxfId="15" priority="17">
       <formula>LEN(TRIM(A4))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M8:N8">
-    <cfRule type="containsBlanks" dxfId="14" priority="12">
-      <formula>LEN(TRIM(M8))=0</formula>
+  <conditionalFormatting sqref="O9:P9">
+    <cfRule type="containsBlanks" dxfId="14" priority="15">
+      <formula>LEN(TRIM(O9))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6:G6 I6:L6 A9 A12">
-    <cfRule type="containsBlanks" dxfId="13" priority="11">
-      <formula>LEN(TRIM(A6))=0</formula>
+  <conditionalFormatting sqref="A7:H7 J7 A10 L7:N7">
+    <cfRule type="containsBlanks" dxfId="13" priority="14">
+      <formula>LEN(TRIM(A7))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M6:N6">
-    <cfRule type="containsBlanks" dxfId="12" priority="10">
-      <formula>LEN(TRIM(M6))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H6">
-    <cfRule type="containsBlanks" dxfId="11" priority="9">
-      <formula>LEN(TRIM(H6))=0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J7">
-    <cfRule type="containsBlanks" dxfId="10" priority="8">
-      <formula>LEN(TRIM(J7))=0</formula>
+  <conditionalFormatting sqref="O7:P7">
+    <cfRule type="containsBlanks" dxfId="12" priority="13">
+      <formula>LEN(TRIM(O7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="containsBlanks" dxfId="9" priority="7">
+    <cfRule type="containsBlanks" dxfId="11" priority="12">
       <formula>LEN(TRIM(I7))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7">
-    <cfRule type="containsBlanks" dxfId="8" priority="6">
-      <formula>LEN(TRIM(H7))=0</formula>
+  <conditionalFormatting sqref="L8">
+    <cfRule type="containsBlanks" dxfId="10" priority="11">
+      <formula>LEN(TRIM(L8))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D11">
-    <cfRule type="containsBlanks" dxfId="7" priority="5">
-      <formula>LEN(TRIM(D11))=0</formula>
+  <conditionalFormatting sqref="J8">
+    <cfRule type="containsBlanks" dxfId="9" priority="10">
+      <formula>LEN(TRIM(J8))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
-    <cfRule type="containsBlanks" dxfId="6" priority="4">
-      <formula>LEN(TRIM(D13))=0</formula>
+  <conditionalFormatting sqref="I8">
+    <cfRule type="containsBlanks" dxfId="8" priority="9">
+      <formula>LEN(TRIM(I8))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J13">
-    <cfRule type="containsBlanks" dxfId="5" priority="3">
-      <formula>LEN(TRIM(J13))=0</formula>
+  <conditionalFormatting sqref="D12:E12">
+    <cfRule type="containsBlanks" dxfId="7" priority="8">
+      <formula>LEN(TRIM(D12))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J10">
-    <cfRule type="containsBlanks" dxfId="4" priority="2">
-      <formula>LEN(TRIM(J10))=0</formula>
+  <conditionalFormatting sqref="D14:E14">
+    <cfRule type="containsBlanks" dxfId="6" priority="7">
+      <formula>LEN(TRIM(D14))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J14">
-    <cfRule type="containsBlanks" dxfId="3" priority="1">
-      <formula>LEN(TRIM(J14))=0</formula>
+  <conditionalFormatting sqref="L14">
+    <cfRule type="containsBlanks" dxfId="5" priority="6">
+      <formula>LEN(TRIM(L14))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L11">
+    <cfRule type="containsBlanks" dxfId="4" priority="5">
+      <formula>LEN(TRIM(L11))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L15">
+    <cfRule type="containsBlanks" dxfId="3" priority="4">
+      <formula>LEN(TRIM(L15))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K9:K15 K4:K6">
+    <cfRule type="containsBlanks" dxfId="2" priority="3">
+      <formula>LEN(TRIM(K4))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K7">
+    <cfRule type="containsBlanks" dxfId="1" priority="2">
+      <formula>LEN(TRIM(K7))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K8">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(K8))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
make the talkcolor logic better
</commit_message>
<xml_diff>
--- a/ConfigData/Xlsx/Quest.xlsx
+++ b/ConfigData/Xlsx/Quest.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TOMClassic\ConfigData\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Code\TOMClassicGit\ConfigData\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -322,14 +322,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>G|乔斯基||让你去找|G|瓦里斯||，并向他学习战斗的技巧，提升自己。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|乔斯基||需要一些罂粟花苗，让你寻找收集一些。应该可以从|O|罂粟花田||中找到。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>狼群的威胁</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -421,18 +413,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>G|塞尼斯||希望你帮助他，进入附近的|O|狼穴||并消灭狼群，如果失败了，你可以尝试反复进出本地图重试。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|塞尼斯||告诉你，再附近的森林深处，有一只神兽|O|穷奇||，如果你可以找到并击败他，会得到丰厚的回报。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
-    <t>G|塞巴斯恰恩||的宠物|G|恰恰||不见了，他希望你可以帮助他找回宠物。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>G|奥莱伊李||觉得目前的田野很不安全，希望你可以帮助他清理当前场景的所有特殊事件。</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -497,10 +477,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>G|奥莱伊李||教了你种植植物的方法，||你需要到附近的田地里，种下|Y|豌豆种子||。并在收获后，把果实带交给他。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>questpickpoppy</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -519,10 +495,6 @@
     <t>questonelesson</t>
   </si>
   <si>
-    <t>G|塞巴斯恰恩||委托你找到可恶的|G|科迪||，并通过卡牌战斗的方式击败他。|G|科迪||经常欺负周边的村民，非常可恶。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>遗迹村落</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -534,10 +506,6 @@
     <t>stonewords</t>
   </si>
   <si>
-    <t>G|科迪||告诉你，附近的|B|村落遗迹||中，隐藏着一些秘密，你可以去调查下，说不定会有意外的收获。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>npckid1</t>
   </si>
   <si>
@@ -552,10 +520,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>G|科迪||希望你可以找到并战胜|B|村落遗迹||中的|O|蛮王之灵||。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>weia</t>
   </si>
   <si>
@@ -583,10 +547,6 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>G|乔斯基||希望你可以去到|B|布萨特高塔||，并在那里历练自己。</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>StartNpcId</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
@@ -637,6 +597,36 @@
   <si>
     <t>eqmuqiang</t>
     <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>G|乔斯基||希望你可以去到|#scene|布萨特高塔||，并在那里历练自己。</t>
+  </si>
+  <si>
+    <t>G|科迪||告诉你，附近的|#scene|村落遗迹||中，隐藏着一些秘密，你可以去调查下，说不定会有意外的收获。</t>
+  </si>
+  <si>
+    <t>G|奥莱伊李||教了你种植植物的方法，||你需要到附近的田地里，种下|#item|豌豆种子||。并在收获后，把果实带交给他。</t>
+  </si>
+  <si>
+    <t>G|塞尼斯||希望你帮助他，进入附近的|#event|狼穴||并消灭狼群，如果失败了，你可以尝试反复进出本地图重试。</t>
+  </si>
+  <si>
+    <t>G|乔斯基||需要一些罂粟花苗，让你寻找收集一些。应该可以从|#event|罂粟花田||中找到。</t>
+  </si>
+  <si>
+    <t>G|塞尼斯||告诉你，再附近的森林深处，有一只神兽|#event|穷奇||，如果你可以找到并击败他，会得到丰厚的回报。</t>
+  </si>
+  <si>
+    <t>G|科迪||希望你可以找到并战胜|#scene|村落遗迹||中的|#event|蛮王之灵||。</t>
+  </si>
+  <si>
+    <t>G|乔斯基||让你去找|#npc|瓦里斯||，并向他学习战斗的技巧，提升自己。</t>
+  </si>
+  <si>
+    <t>G|塞巴斯恰恩||的宠物|#npc|恰恰||不见了，他希望你可以帮助他找回宠物。</t>
+  </si>
+  <si>
+    <t>G|塞巴斯恰恩||委托你找到可恶的|#npc|科迪||，并通过卡牌战斗的方式击败他。|#npc|科迪||经常欺负周边的村民，非常可恶。</t>
   </si>
 </sst>
 </file>
@@ -1547,6 +1537,74 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1609,7 +1667,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1924,8 +1982,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1957,7 +2015,7 @@
         <v>54</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>7</v>
@@ -1972,10 +2030,10 @@
         <v>2</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="L1" s="22" t="s">
         <v>33</v>
@@ -1984,28 +2042,28 @@
         <v>36</v>
       </c>
       <c r="N1" s="22" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="O1" s="23" t="s">
         <v>48</v>
       </c>
       <c r="P1" s="23" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="Q1" s="23" t="s">
         <v>52</v>
       </c>
       <c r="R1" s="24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="S1" s="25" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="T1" s="26" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="U1" s="26" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="V1" s="27" t="s">
         <v>9</v>
@@ -2029,7 +2087,7 @@
         <v>23</v>
       </c>
       <c r="AC1" s="27" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="AD1" s="27" t="s">
         <v>14</v>
@@ -2052,7 +2110,7 @@
         <v>55</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>6</v>
@@ -2073,7 +2131,7 @@
         <v>0</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>37</v>
@@ -2085,19 +2143,19 @@
         <v>17</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="Q2" s="9" t="s">
         <v>17</v>
       </c>
       <c r="R2" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="S2" s="16" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="U2" s="7" t="s">
         <v>0</v>
@@ -2147,7 +2205,7 @@
         <v>56</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>8</v>
@@ -2162,40 +2220,40 @@
         <v>5</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="O3" s="10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P3" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="Q3" s="10" t="s">
         <v>53</v>
       </c>
       <c r="R3" s="12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="S3" s="12" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="T3" s="17" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="U3" s="17" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="V3" s="2" t="s">
         <v>18</v>
@@ -2213,10 +2271,10 @@
         <v>20</v>
       </c>
       <c r="AA3" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="AC3" s="2" t="s">
         <v>26</v>
@@ -2225,7 +2283,7 @@
         <v>21</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.15">
@@ -2248,25 +2306,25 @@
         <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>57</v>
+        <v>136</v>
       </c>
       <c r="J4">
         <v>42120001</v>
       </c>
       <c r="L4" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M4" s="8" t="s">
         <v>38</v>
       </c>
       <c r="N4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="P4">
         <v>10</v>
       </c>
       <c r="R4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="V4">
         <v>100</v>
@@ -2280,10 +2338,10 @@
         <v>12000002</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C5" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="D5">
         <v>12000001</v>
@@ -2298,7 +2356,7 @@
         <v>7</v>
       </c>
       <c r="I5" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="J5">
         <v>42120001</v>
@@ -2307,7 +2365,7 @@
         <v>42130031</v>
       </c>
       <c r="L5" s="18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
@@ -2325,10 +2383,10 @@
         <v>12000003</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -2340,29 +2398,29 @@
         <v>4</v>
       </c>
       <c r="I6" t="s">
-        <v>83</v>
+        <v>132</v>
       </c>
       <c r="J6">
         <v>42120002</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M6" s="8"/>
       <c r="P6">
         <v>5</v>
       </c>
       <c r="R6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="Z6">
         <v>100</v>
       </c>
       <c r="AA6" s="28" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="AB6" s="19" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.15">
@@ -2385,25 +2443,25 @@
         <v>5</v>
       </c>
       <c r="I7" t="s">
-        <v>85</v>
+        <v>137</v>
       </c>
       <c r="J7">
         <v>42120003</v>
       </c>
       <c r="L7" s="13" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="M7" s="8" t="s">
         <v>38</v>
       </c>
       <c r="N7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="P7">
         <v>10</v>
       </c>
       <c r="R7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="V7">
         <v>100</v>
@@ -2432,19 +2490,19 @@
         <v>3</v>
       </c>
       <c r="I8" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J8">
         <v>42120005</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="S8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="V8">
         <v>100</v>
@@ -2453,7 +2511,7 @@
         <v>100</v>
       </c>
       <c r="AA8" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.15">
@@ -2461,10 +2519,10 @@
         <v>12000007</v>
       </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -2476,13 +2534,13 @@
         <v>3</v>
       </c>
       <c r="I9" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J9">
         <v>42120014</v>
       </c>
       <c r="L9" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
@@ -2490,7 +2548,7 @@
         <v>10</v>
       </c>
       <c r="R9" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="V9">
         <v>100</v>
@@ -2504,10 +2562,10 @@
         <v>12000010</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -2519,13 +2577,13 @@
         <v>5</v>
       </c>
       <c r="I10" t="s">
-        <v>112</v>
+        <v>130</v>
       </c>
       <c r="J10">
         <v>42120006</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
@@ -2533,7 +2591,7 @@
         <v>10</v>
       </c>
       <c r="R10" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="V10">
         <v>100</v>
@@ -2568,13 +2626,13 @@
         <v>1</v>
       </c>
       <c r="I11" t="s">
-        <v>58</v>
+        <v>133</v>
       </c>
       <c r="J11">
         <v>42120001</v>
       </c>
       <c r="L11" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -2585,7 +2643,7 @@
         <v>10</v>
       </c>
       <c r="Q11" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="V11">
         <v>50</v>
@@ -2599,10 +2657,10 @@
         <v>12000102</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C12" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D12">
         <v>12000003</v>
@@ -2620,13 +2678,13 @@
         <v>6</v>
       </c>
       <c r="I12" t="s">
-        <v>84</v>
+        <v>134</v>
       </c>
       <c r="J12">
         <v>42120002</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
@@ -2634,7 +2692,7 @@
         <v>10</v>
       </c>
       <c r="R12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="V12">
         <v>300</v>
@@ -2649,10 +2707,10 @@
         <v>85</v>
       </c>
       <c r="AA12" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="AB12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.15">
@@ -2660,10 +2718,10 @@
         <v>12000103</v>
       </c>
       <c r="B13" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D13">
         <v>12000006</v>
@@ -2681,18 +2739,18 @@
         <v>2</v>
       </c>
       <c r="I13" t="s">
-        <v>102</v>
+        <v>131</v>
       </c>
       <c r="J13">
         <v>42120005</v>
       </c>
       <c r="L13" s="18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
       <c r="T13" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="Z13">
         <v>50</v>
@@ -2704,10 +2762,10 @@
         <v>12000104</v>
       </c>
       <c r="B14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C14" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D14">
         <v>12000005</v>
@@ -2725,24 +2783,24 @@
         <v>7</v>
       </c>
       <c r="I14" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="J14">
         <v>42120003</v>
       </c>
       <c r="L14" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
       <c r="O14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="P14">
         <v>10</v>
       </c>
       <c r="Q14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="V14">
         <v>50</v>
@@ -2751,7 +2809,7 @@
         <v>50</v>
       </c>
       <c r="AE14" s="19" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.15">
@@ -2759,10 +2817,10 @@
         <v>12000105</v>
       </c>
       <c r="B15" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C15" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D15">
         <v>12000010</v>
@@ -2780,13 +2838,13 @@
         <v>8</v>
       </c>
       <c r="I15" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
       <c r="J15">
         <v>42120006</v>
       </c>
       <c r="L15" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
@@ -2794,7 +2852,7 @@
         <v>10</v>
       </c>
       <c r="R15" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="V15">
         <v>300</v>

</xml_diff>